<commit_message>
test Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -13,23 +13,134 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>SimpleRules Boolean test(IntValue param)</t>
+  </si>
+  <si>
+    <t>param</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color rgb="000001"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -37,11 +148,498 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -344,12 +942,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s" s="6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update table Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>SimpleRules Boolean test(IntValue param)</t>
   </si>
@@ -615,7 +615,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -942,7 +942,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C6"/>
+  <dimension ref="B3:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -978,6 +978,30 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" s="5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C7" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C9" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
Create listsCardsByClient Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>SimpleRules Boolean test(IntValue param)</t>
   </si>
@@ -35,6 +35,129 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>SimpleRules String listsCardsByClient(String situation, DoubleRange income)</t>
+  </si>
+  <si>
+    <t>situation</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>&lt;=1000000</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>1000001 .. 2000000</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>2000001 .. 3000000</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>&gt;=3000001</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>&lt;=100000</t>
+  </si>
+  <si>
+    <t>TC1T</t>
+  </si>
+  <si>
+    <t>&gt;=1000001</t>
+  </si>
+  <si>
+    <t>TC2T</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>&lt;=2000000</t>
+  </si>
+  <si>
+    <t>TC1I</t>
+  </si>
+  <si>
+    <t>2000001 .. 4000000</t>
+  </si>
+  <si>
+    <t>TCI2</t>
+  </si>
+  <si>
+    <t>4000001 .. 6000000</t>
+  </si>
+  <si>
+    <t>TCI3</t>
+  </si>
+  <si>
+    <t>6000001 .. 8000000</t>
+  </si>
+  <si>
+    <t>Test listsCardsByClient listsCardsByClientTest</t>
+  </si>
+  <si>
+    <t>Situation</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>2000000</t>
+  </si>
+  <si>
+    <t>200000</t>
+  </si>
+  <si>
+    <t>0 .. 1000000</t>
+  </si>
+  <si>
+    <t>SimpleRules String listsCardsByClient(String situation, DoubleValue income)</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>TCP1</t>
+  </si>
+  <si>
+    <t>&lt;=300000</t>
+  </si>
+  <si>
+    <t>TCP2</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>&lt;=10000000</t>
+  </si>
+  <si>
+    <t>TCO1</t>
   </si>
 </sst>
 </file>
@@ -42,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -89,6 +212,207 @@
       <name val="&quot;Franklin Gothik Book&quot;"/>
       <sz val="10.0"/>
       <color rgb="000001"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
       <u val="none"/>
     </font>
   </fonts>
@@ -140,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -613,11 +937,29 @@
         <color rgb="000001"/>
       </bottom>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
@@ -641,6 +983,110 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -942,7 +1388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C9"/>
+  <dimension ref="B3:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -1002,9 +1448,172 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11">
+      <c r="B11" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s" s="15">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s" s="16">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s" s="17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="18">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s" s="20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s" s="21">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s" s="23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s" s="25">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s" s="27">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s" s="28">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s" s="30">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s" s="31">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s" s="32">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s" s="33">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s" s="34">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s" s="35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s" s="36">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s" s="37">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s" s="38">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s" s="39">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s" s="40">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s" s="41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Data created Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>SimpleRules Boolean test(IntValue param)</t>
   </si>
@@ -158,6 +158,36 @@
   </si>
   <si>
     <t>TCO1</t>
+  </si>
+  <si>
+    <t>Data String test12</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Datatype test1</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Data String EmployeeSituation</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Fijo</t>
+  </si>
+  <si>
+    <t>Identificacion</t>
   </si>
 </sst>
 </file>
@@ -959,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
@@ -1086,6 +1116,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1388,7 +1422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D26"/>
+  <dimension ref="B3:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -1610,6 +1644,38 @@
       </c>
     </row>
     <row r="26"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="39">
+      <c r="B39" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s" s="48">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
Project BBVA_Rules is saved. Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>SimpleRules Boolean test(IntValue param)</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>Identificacion</t>
+  </si>
+  <si>
+    <t>Datatype EmployeeSituation</t>
+  </si>
+  <si>
+    <t>EmployeeSituation</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
@@ -1116,6 +1122,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
@@ -1422,7 +1429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D41"/>
+  <dimension ref="B3:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -1676,10 +1683,33 @@
         <v>57</v>
       </c>
     </row>
+    <row r="43">
+      <c r="B43" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="49"/>
+    </row>
+    <row r="44">
+      <c r="B44" t="s" s="49">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s" s="49">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s" s="49">
+        <v>52</v>
+      </c>
+      <c r="C45" t="s" s="49">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B43:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Return BinCards on suggestCard + Employee Situation Data Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="138">
   <si>
     <t>SimpleRules Boolean test(IntValue param)</t>
   </si>
@@ -194,6 +194,240 @@
   </si>
   <si>
     <t>EmployeeSituation</t>
+  </si>
+  <si>
+    <t>Data EmployeeSituation Situation</t>
+  </si>
+  <si>
+    <t>EMPLOYEESITUATION</t>
+  </si>
+  <si>
+    <t>Independiente</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>SimpleRules String jklhlkjhlkj(EmployeeSituation id, String field)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>Temporal</t>
+  </si>
+  <si>
+    <t>Pensionado</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>Data EmployeeSituation EmployeeSituationData</t>
+  </si>
+  <si>
+    <t>SimpleRules String test2(EmployeeSituation employeeSituation, BigDecimalValue income)</t>
+  </si>
+  <si>
+    <t>employeeSituation</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>_ID_</t>
+  </si>
+  <si>
+    <t>_NAME_</t>
+  </si>
+  <si>
+    <t>Data String EmployeeSituationList</t>
+  </si>
+  <si>
+    <t>Data EmployeeSituation EmployeeSituationList</t>
+  </si>
+  <si>
+    <t>SimpleRules String prueba(EmployeeSituation ES, Integer income)</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>I,Independiente</t>
+  </si>
+  <si>
+    <t>(I,Independiente)</t>
+  </si>
+  <si>
+    <t>('I',Independiente)</t>
+  </si>
+  <si>
+    <t>EmployeeSituation('I')</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&gt; EmployeeSituation</t>
+  </si>
+  <si>
+    <t>&lt;P&gt;</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>F,Fijo</t>
+  </si>
+  <si>
+    <t>(F,Fijo)</t>
+  </si>
+  <si>
+    <t>(Fijo)</t>
+  </si>
+  <si>
+    <t>SimpleRules String popopopo(EmployeeSituation[] aa, Integer kjhkjhk)</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>kjhkjhk</t>
+  </si>
+  <si>
+    <t>I,F,P</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>qweqwe</t>
+  </si>
+  <si>
+    <t>I;F;P</t>
+  </si>
+  <si>
+    <t>SimpleRules String popopopo(EmployeeSituation aa, Integer kjhkjhk)</t>
+  </si>
+  <si>
+    <t>SimpleRules String suggestCardsBy(String situation, DoubleValue income)</t>
+  </si>
+  <si>
+    <t>SimpleRules String suggestCards(String situation, DoubleValue income)</t>
+  </si>
+  <si>
+    <t>Datatype binCard</t>
+  </si>
+  <si>
+    <t>_BIN_</t>
+  </si>
+  <si>
+    <t>_FRANCHISE_</t>
+  </si>
+  <si>
+    <t>Data binCard binCardList</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
+  <si>
+    <t>franchise</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>421892</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Visa Congelada</t>
+  </si>
+  <si>
+    <t>450407</t>
+  </si>
+  <si>
+    <t>Visa Studio F</t>
+  </si>
+  <si>
+    <t>518761</t>
+  </si>
+  <si>
+    <t>Mastercard</t>
+  </si>
+  <si>
+    <t>Mastercard Standard World Vision</t>
+  </si>
+  <si>
+    <t>450408</t>
+  </si>
+  <si>
+    <t>Visa Oro</t>
+  </si>
+  <si>
+    <t>518841</t>
+  </si>
+  <si>
+    <t>Mastercard Gold World Vision</t>
+  </si>
+  <si>
+    <t>459418</t>
+  </si>
+  <si>
+    <t>Mastercard Platinum</t>
+  </si>
+  <si>
+    <t>404280</t>
+  </si>
+  <si>
+    <t>Visa Platinum</t>
+  </si>
+  <si>
+    <t>548115</t>
+  </si>
+  <si>
+    <t>459419</t>
+  </si>
+  <si>
+    <t>Visa Avianca Lifemiles Platinum</t>
+  </si>
+  <si>
+    <t>553643</t>
+  </si>
+  <si>
+    <t>Mastercard Black</t>
+  </si>
+  <si>
+    <t>553643, 459419</t>
+  </si>
+  <si>
+    <t>450408, 518841</t>
+  </si>
+  <si>
+    <t>450408;518841</t>
+  </si>
+  <si>
+    <t>553643;459419</t>
+  </si>
+  <si>
+    <t>421892;450408;518761</t>
+  </si>
+  <si>
+    <t>450407;421892;450408;518761</t>
+  </si>
+  <si>
+    <t>Mastercard Platinum Elite</t>
   </si>
 </sst>
 </file>
@@ -201,7 +435,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="65" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -431,6 +665,162 @@
       <name val="&quot;Franklin Gothik Book&quot;"/>
       <sz val="10.0"/>
       <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
       <u val="none"/>
     </font>
     <font>
@@ -500,7 +890,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -991,11 +1381,20 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
@@ -1125,6 +1524,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="53" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
@@ -1429,69 +1927,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D45"/>
+  <dimension ref="B3:D112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3">
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4">
-      <c r="B4" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C7" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C8" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C9" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
     <row r="11">
       <c r="B11" s="42" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="42"/>
@@ -1514,8 +1965,8 @@
       <c r="C13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s" s="14">
-        <v>12</v>
+      <c r="D13" s="14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="14">
@@ -1525,8 +1976,8 @@
       <c r="C14" t="s" s="16">
         <v>13</v>
       </c>
-      <c r="D14" t="s" s="17">
-        <v>14</v>
+      <c r="D14" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15">
@@ -1536,8 +1987,8 @@
       <c r="C15" t="s" s="19">
         <v>15</v>
       </c>
-      <c r="D15" t="s" s="20">
-        <v>16</v>
+      <c r="D15" s="20" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16">
@@ -1547,8 +1998,8 @@
       <c r="C16" t="s" s="22">
         <v>17</v>
       </c>
-      <c r="D16" t="s" s="23">
-        <v>18</v>
+      <c r="D16" s="23" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="17">
@@ -1558,8 +2009,8 @@
       <c r="C17" t="s" s="25">
         <v>20</v>
       </c>
-      <c r="D17" t="s" s="26">
-        <v>21</v>
+      <c r="D17" s="26" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="18">
@@ -1569,8 +2020,8 @@
       <c r="C18" t="s" s="28">
         <v>22</v>
       </c>
-      <c r="D18" t="s" s="29">
-        <v>23</v>
+      <c r="D18" s="29" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="19">
@@ -1580,8 +2031,8 @@
       <c r="C19" t="s" s="31">
         <v>25</v>
       </c>
-      <c r="D19" t="s" s="32">
-        <v>26</v>
+      <c r="D19" s="32" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="20">
@@ -1591,8 +2042,8 @@
       <c r="C20" t="s" s="34">
         <v>27</v>
       </c>
-      <c r="D20" t="s" s="35">
-        <v>28</v>
+      <c r="D20" s="35" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="21">
@@ -1602,8 +2053,8 @@
       <c r="C21" t="s" s="37">
         <v>29</v>
       </c>
-      <c r="D21" t="s" s="38">
-        <v>30</v>
+      <c r="D21" s="38" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22">
@@ -1613,8 +2064,8 @@
       <c r="C22" t="s" s="40">
         <v>31</v>
       </c>
-      <c r="D22" t="s" s="41">
-        <v>30</v>
+      <c r="D22" s="41" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="23">
@@ -1625,7 +2076,7 @@
         <v>43</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24">
@@ -1647,7 +2098,7 @@
         <v>46</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26"/>
@@ -1683,33 +2134,279 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43">
-      <c r="B43" s="49" t="s">
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="67">
+      <c r="B67" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="49"/>
-    </row>
-    <row r="44">
-      <c r="B44" t="s" s="49">
+      <c r="C67" s="67"/>
+    </row>
+    <row r="68">
+      <c r="B68" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="C44" t="s" s="49">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="s" s="49">
+      <c r="C68" t="s" s="67">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="C45" t="s" s="49">
-        <v>59</v>
+      <c r="C69" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="75">
+      <c r="B75" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="69"/>
+    </row>
+    <row r="76">
+      <c r="B76" t="s" s="69">
+        <v>76</v>
+      </c>
+      <c r="C76" t="s" s="69">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="69" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" s="69" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="C80" s="69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C81" s="69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="92">
+      <c r="B92" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="C92" s="88"/>
+    </row>
+    <row r="93">
+      <c r="B93" t="s" s="88">
+        <v>52</v>
+      </c>
+      <c r="C93" t="s" s="88">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s" s="88">
+        <v>52</v>
+      </c>
+      <c r="C94" t="s" s="88">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s" s="88">
+        <v>52</v>
+      </c>
+      <c r="C95" t="s" s="88">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="101">
+      <c r="B101" s="90" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" s="90"/>
+      <c r="D101" s="90"/>
+    </row>
+    <row r="102">
+      <c r="B102" t="s" s="90">
+        <v>104</v>
+      </c>
+      <c r="C102" t="s" s="90">
+        <v>105</v>
+      </c>
+      <c r="D102" t="s" s="90">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="C103" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="D103" s="90" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" s="90" t="s">
+        <v>113</v>
+      </c>
+      <c r="C104" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="D104" s="90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" s="90" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="D105" s="90" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" s="90" t="s">
+        <v>118</v>
+      </c>
+      <c r="C106" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="D106" s="90" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="C107" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="D107" s="90" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="C108" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="D108" s="90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" s="90" t="s">
+        <v>124</v>
+      </c>
+      <c r="C109" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="D109" s="90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" s="90" t="s">
+        <v>126</v>
+      </c>
+      <c r="C110" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="D110" s="90" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" s="90" t="s">
+        <v>127</v>
+      </c>
+      <c r="C111" s="90" t="s">
+        <v>111</v>
+      </c>
+      <c r="D111" s="90" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" s="90" t="s">
+        <v>129</v>
+      </c>
+      <c r="C112" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="D112" s="90" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:C3"/>
+  <mergeCells count="6">
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B101:D101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change response suggestCards Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="142">
   <si>
     <t>SimpleRules Boolean test(IntValue param)</t>
   </si>
@@ -428,6 +428,18 @@
   </si>
   <si>
     <t>Mastercard Platinum Elite</t>
+  </si>
+  <si>
+    <t>421892,450408,518761</t>
+  </si>
+  <si>
+    <t>450407,421892,450408,518761</t>
+  </si>
+  <si>
+    <t>450408,518841</t>
+  </si>
+  <si>
+    <t>553643,459419</t>
   </si>
 </sst>
 </file>
@@ -1999,7 +2011,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17">
@@ -2043,7 +2055,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21">
@@ -2054,7 +2066,7 @@
         <v>29</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22">
@@ -2065,7 +2077,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23">
@@ -2076,7 +2088,7 @@
         <v>43</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24">
@@ -2087,7 +2099,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">

</xml_diff>

<commit_message>
create ratio score TRANS Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="157">
   <si>
     <t>SimpleRules Boolean test(IntValue param)</t>
   </si>
@@ -440,6 +440,51 @@
   </si>
   <si>
     <t>553643,459419</t>
+  </si>
+  <si>
+    <t>SimpleRules DoubleValue ratioScoreTransunion(DoubleRange ratio)</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>&lt;=10</t>
+  </si>
+  <si>
+    <t>(10 .. 15]</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>(15 .. 20]</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>(20 .. 30]</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>(30 .. 40]</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>(40 .. 150]</t>
+  </si>
+  <si>
+    <t>&gt;150</t>
+  </si>
+  <si>
+    <t>SimpleRules DoubleValue ratioScore_TRANS(DoubleRange ratio)</t>
+  </si>
+  <si>
+    <t>SimpleRules DoubleValue ratioScore_TRANS(DoubleValue ratio)</t>
   </si>
 </sst>
 </file>
@@ -447,7 +492,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="65" x14ac:knownFonts="1">
+  <fonts count="81" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -833,6 +878,104 @@
       <sz val="10.0"/>
       <color indexed="8"/>
       <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
       <u val="none"/>
     </font>
     <font>
@@ -1406,7 +1549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
@@ -1638,6 +1781,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="65" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1939,7 +2134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D112"/>
+  <dimension ref="B3:D122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -2412,6 +2607,76 @@
         <v>130</v>
       </c>
     </row>
+    <row r="114">
+      <c r="B114" s="107" t="s">
+        <v>156</v>
+      </c>
+      <c r="C114" s="107"/>
+    </row>
+    <row r="115">
+      <c r="B115" t="s" s="91">
+        <v>143</v>
+      </c>
+      <c r="C115" t="s" s="92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" t="s" s="93">
+        <v>144</v>
+      </c>
+      <c r="C116" t="s" s="94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" t="s" s="95">
+        <v>145</v>
+      </c>
+      <c r="C117" t="s" s="96">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" t="s" s="97">
+        <v>147</v>
+      </c>
+      <c r="C118" t="s" s="98">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" t="s" s="99">
+        <v>149</v>
+      </c>
+      <c r="C119" t="s" s="100">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" t="s" s="101">
+        <v>151</v>
+      </c>
+      <c r="C120" t="s" s="102">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" t="s" s="103">
+        <v>153</v>
+      </c>
+      <c r="C121" t="s" s="104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" t="s" s="105">
+        <v>154</v>
+      </c>
+      <c r="C122" t="s" s="106">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B11:D11"/>
@@ -2419,6 +2684,7 @@
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B92:C92"/>
     <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B114:C114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
suggestCards3 temp Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCCF09C-9E6C-EE47-87FE-0761B2B2DE16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A5136-7456-904A-B1C9-F823FC8D2808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="135">
   <si>
     <t>RETURN</t>
   </si>
@@ -358,76 +359,73 @@
     <t>R13</t>
   </si>
   <si>
-    <t>Rules String [] suggestCards2(String situation, DoubleValue income)</t>
-  </si>
-  <si>
-    <t>DoubleValue</t>
-  </si>
-  <si>
-    <t>(0 .. 1000000]</t>
-  </si>
-  <si>
-    <t>(1000001 .. 2000000]</t>
-  </si>
-  <si>
-    <t>(2000001 .. 3000000]</t>
-  </si>
-  <si>
-    <t>(2000001 .. 4000000]</t>
-  </si>
-  <si>
-    <t>(4000001 .. 6000000]</t>
-  </si>
-  <si>
-    <t>(6000001 .. 8000000]</t>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>DoubleRange</t>
+  </si>
+  <si>
+    <t>Rules String[] suggestCards2(String situation, DoubleRange income)</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>Double min</t>
+  </si>
+  <si>
+    <t>Double max</t>
+  </si>
+  <si>
+    <t>Desde</t>
+  </si>
+  <si>
+    <t>Hasta</t>
+  </si>
+  <si>
+    <t>Objeto</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Rules String[] suggestCards3 (String situation, DoubleValue income)</t>
+  </si>
+  <si>
+    <t>income &lt;= max</t>
+  </si>
+  <si>
+    <t>min &lt;= income</t>
+  </si>
+  <si>
+    <t>sit = situation</t>
+  </si>
+  <si>
+    <t>String sit</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>situation = sit</t>
+  </si>
+  <si>
+    <t>Rules String[] suggestCards3 (String situation, Double income)</t>
   </si>
   <si>
     <t>Situation</t>
   </si>
   <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Double</t>
-  </si>
-  <si>
-    <t>Rules String [] suggestCards2(String situation, Double income)</t>
-  </si>
-  <si>
-    <t>Test suggestCards2 suggestCards2Test</t>
-  </si>
-  <si>
-    <t>_res_</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>SimpleRules String [] suggestCards2(String situation, Double income)</t>
-  </si>
-  <si>
-    <t>(1000001 .... 2000000]</t>
-  </si>
-  <si>
-    <t>SimpleRules String [] suggestCards2(String situation, DoubleRange income)</t>
-  </si>
-  <si>
-    <t>DoubleRange</t>
-  </si>
-  <si>
-    <t>SimpleRules String[] suggestCards2(String situation, DoubleRange income)</t>
-  </si>
-  <si>
-    <t>Rules String[] suggestCards2(String situation, DoubleRange income)</t>
-  </si>
-  <si>
-    <t>Rules String[] suggestCards2(String situation, DoubleValue income)</t>
-  </si>
-  <si>
-    <t>SinpleRules String[] suggestCards2(String situation, DoubleValue income)</t>
-  </si>
-  <si>
-    <t>SimpleRules String[] suggestCards2(String situation, DoubleValue income)</t>
+    <t>IncomeIni</t>
+  </si>
+  <si>
+    <t>IncomeOut</t>
   </si>
 </sst>
 </file>
@@ -435,7 +433,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="59">
+  <fonts count="60">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -740,6 +738,12 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="&quot;Franklin Gothik Book&quot;"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -770,21 +774,25 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="0"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -889,61 +897,19 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
       <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="0"/>
+        <color auto="1"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
-        <color indexed="0"/>
+        <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -958,12 +924,13 @@
       <bottom style="thin">
         <color indexed="0"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1119,23 +1086,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="58" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1144,19 +1097,56 @@
     <xf numFmtId="0" fontId="58" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="58" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="58" fillId="8" borderId="18" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="58" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1496,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:E171"/>
+  <dimension ref="B4:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView topLeftCell="A137" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E149" sqref="E149:E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1511,11 +1501,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
@@ -1696,10 +1686,10 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="58" t="s">
+      <c r="B60" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="58"/>
+      <c r="C60" s="73"/>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="35" t="s">
@@ -1718,10 +1708,10 @@
       </c>
     </row>
     <row r="68" spans="2:3">
-      <c r="B68" s="58" t="s">
+      <c r="B68" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C68" s="58"/>
+      <c r="C68" s="73"/>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="36" t="s">
@@ -1772,10 +1762,10 @@
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85" s="58" t="s">
+      <c r="B85" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="58"/>
+      <c r="C85" s="73"/>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" s="37" t="s">
@@ -1802,11 +1792,11 @@
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="B94" s="58" t="s">
+      <c r="B94" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="C94" s="58"/>
-      <c r="D94" s="58"/>
+      <c r="C94" s="73"/>
+      <c r="D94" s="73"/>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" s="38" t="s">
@@ -1930,10 +1920,10 @@
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="57" t="s">
+      <c r="B107" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="57"/>
+      <c r="C107" s="71"/>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="39" t="s">
@@ -2000,13 +1990,13 @@
       </c>
     </row>
     <row r="117" spans="2:5">
-      <c r="B117" s="59" t="s">
+      <c r="B117" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="C117" s="58"/>
+      <c r="C117" s="73"/>
     </row>
     <row r="118" spans="2:5">
-      <c r="B118" s="60" t="s">
+      <c r="B118" s="57" t="s">
         <v>81</v>
       </c>
       <c r="C118" s="56" t="s">
@@ -2014,440 +2004,455 @@
       </c>
     </row>
     <row r="127" spans="2:5">
-      <c r="B127" s="63" t="s">
+      <c r="B127" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="C127" s="63"/>
-      <c r="D127" s="63"/>
-      <c r="E127" s="63"/>
+      <c r="C127" s="74"/>
+      <c r="D127" s="74"/>
+      <c r="E127" s="74"/>
     </row>
     <row r="128" spans="2:5" ht="18">
-      <c r="B128" s="61" t="s">
+      <c r="B128" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C128" s="61" t="s">
+      <c r="C128" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="D128" s="61" t="s">
+      <c r="D128" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="E128" s="61" t="s">
+      <c r="E128" s="58" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="129" spans="2:5" ht="18">
-      <c r="B129" s="62"/>
-      <c r="C129" s="62" t="s">
+      <c r="B129" s="59"/>
+      <c r="C129" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="D129" s="62" t="s">
+      <c r="D129" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="E129" s="62"/>
+      <c r="E129" s="59"/>
     </row>
     <row r="130" spans="2:5" ht="18">
-      <c r="B130" s="62"/>
-      <c r="C130" s="62" t="s">
+      <c r="B130" s="59"/>
+      <c r="C130" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="D130" s="62" t="s">
+      <c r="D130" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="E130" s="62"/>
+      <c r="E130" s="59"/>
     </row>
     <row r="131" spans="2:5" ht="18">
-      <c r="B131" s="62" t="s">
+      <c r="B131" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="C131" s="62" t="s">
+      <c r="C131" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="D131" s="62" t="s">
+      <c r="D131" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E131" s="62" t="s">
+      <c r="E131" s="59" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="132" spans="2:5" ht="18">
-      <c r="B132" s="62" t="s">
+      <c r="B132" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C132" s="62" t="s">
+      <c r="C132" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="D132" s="62">
+      <c r="D132" s="59">
         <v>1</v>
       </c>
-      <c r="E132" s="62" t="s">
+      <c r="E132" s="59" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="133" spans="2:5" s="55" customFormat="1" ht="18">
-      <c r="B133" s="64" t="s">
+      <c r="B133" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="C133" s="64" t="s">
+      <c r="C133" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="D133" s="64">
+      <c r="D133" s="69">
         <v>1</v>
       </c>
-      <c r="E133" s="62" t="s">
+      <c r="E133" s="59" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="134" spans="2:5" ht="18">
-      <c r="B134" s="64"/>
-      <c r="C134" s="64"/>
-      <c r="D134" s="64"/>
-      <c r="E134" s="62" t="s">
+      <c r="B134" s="69"/>
+      <c r="C134" s="69"/>
+      <c r="D134" s="69"/>
+      <c r="E134" s="59" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="135" spans="2:5" ht="18">
-      <c r="B135" s="62" t="s">
+      <c r="B135" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C135" s="62" t="s">
+      <c r="C135" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="D135" s="62">
+      <c r="D135" s="59">
         <v>1</v>
       </c>
-      <c r="E135" s="62" t="s">
+      <c r="E135" s="59" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="136" spans="2:5" ht="18">
-      <c r="B136" s="62" t="s">
+      <c r="B136" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="C136" s="62" t="s">
+      <c r="C136" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="D136" s="62">
+      <c r="D136" s="59">
         <v>1</v>
       </c>
-      <c r="E136" s="62" t="s">
+      <c r="E136" s="59" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="141" spans="2:5" ht="15">
-      <c r="B141" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="C141" s="65"/>
-      <c r="D141" s="65"/>
-      <c r="E141" s="65"/>
+      <c r="B141" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="C141" s="70"/>
+      <c r="D141" s="70"/>
+      <c r="E141" s="70"/>
     </row>
     <row r="142" spans="2:5" ht="14">
-      <c r="B142" s="66" t="s">
+      <c r="B142" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="C142" s="66" t="s">
+      <c r="C142" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="D142" s="66" t="s">
+      <c r="D142" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="E142" s="66" t="s">
+      <c r="E142" s="60" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="143" spans="2:5" ht="14">
-      <c r="B143" s="67"/>
-      <c r="C143" s="67" t="s">
+      <c r="B143" s="61"/>
+      <c r="C143" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="D143" s="67" t="s">
+      <c r="D143" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E143" s="67"/>
+      <c r="E143" s="61"/>
     </row>
     <row r="144" spans="2:5" ht="14">
-      <c r="B144" s="67"/>
-      <c r="C144" s="67" t="s">
+      <c r="B144" s="61"/>
+      <c r="C144" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="D144" s="67" t="s">
-        <v>130</v>
-      </c>
-      <c r="E144" s="67"/>
+      <c r="D144" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="E144" s="61"/>
     </row>
     <row r="145" spans="2:5" ht="14">
-      <c r="B145" s="67" t="s">
+      <c r="B145" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="C145" s="67" t="s">
+      <c r="C145" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="D145" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="E145" s="67" t="s">
+      <c r="D145" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E145" s="61" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="146" spans="2:5" ht="15">
-      <c r="B146" s="71" t="s">
+      <c r="B146" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C146" s="74" t="s">
+      <c r="C146" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D146" s="68" t="s">
+      <c r="D146" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="E146" s="69" t="s">
+      <c r="E146" s="63" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="147" spans="2:5" ht="15">
-      <c r="B147" s="71" t="s">
+      <c r="B147" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C147" s="74" t="s">
+      <c r="C147" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="D147" s="68" t="s">
+      <c r="D147" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E147" s="69" t="s">
+      <c r="E147" s="63" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="148" spans="2:5" ht="15">
-      <c r="B148" s="71" t="s">
+      <c r="B148" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C148" s="68" t="s">
+      <c r="C148" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D148" s="68" t="s">
+      <c r="D148" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E148" s="69" t="s">
+      <c r="E148" s="63" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="149" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B149" s="72" t="s">
+      <c r="B149" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="C149" s="70" t="s">
+      <c r="C149" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="D149" s="70" t="s">
+      <c r="D149" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="E149" s="69">
+      <c r="E149" s="63">
         <v>421892</v>
       </c>
     </row>
     <row r="150" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B150" s="72"/>
-      <c r="C150" s="70"/>
-      <c r="D150" s="70"/>
-      <c r="E150" s="69">
+      <c r="B150" s="68"/>
+      <c r="C150" s="67"/>
+      <c r="D150" s="67"/>
+      <c r="E150" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="151" spans="2:5" ht="15">
-      <c r="B151" s="72"/>
-      <c r="C151" s="70"/>
-      <c r="D151" s="70"/>
-      <c r="E151" s="69">
+      <c r="B151" s="68"/>
+      <c r="C151" s="67"/>
+      <c r="D151" s="67"/>
+      <c r="E151" s="63">
         <v>518761</v>
       </c>
     </row>
     <row r="152" spans="2:5" ht="15">
-      <c r="B152" s="71" t="s">
+      <c r="B152" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="C152" s="68" t="s">
+      <c r="C152" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D152" s="68" t="s">
+      <c r="D152" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E152" s="69" t="s">
+      <c r="E152" s="63" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="153" spans="2:5" ht="15">
-      <c r="B153" s="71" t="s">
+      <c r="B153" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="C153" s="68" t="s">
+      <c r="C153" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D153" s="68" t="s">
+      <c r="D153" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E153" s="69" t="s">
+      <c r="E153" s="63" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="154" spans="2:5" ht="15">
-      <c r="B154" s="71" t="s">
+      <c r="B154" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="C154" s="68" t="s">
+      <c r="C154" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D154" s="68" t="s">
+      <c r="D154" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="E154" s="69" t="s">
+      <c r="E154" s="63" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="155" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B155" s="72" t="s">
+      <c r="B155" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="C155" s="70" t="s">
+      <c r="C155" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D155" s="68" t="s">
+      <c r="D155" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="E155" s="69">
+      <c r="E155" s="63">
         <v>518761</v>
       </c>
     </row>
     <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B156" s="72"/>
-      <c r="C156" s="70"/>
-      <c r="D156" s="70"/>
-      <c r="E156" s="69">
+      <c r="B156" s="68"/>
+      <c r="C156" s="67"/>
+      <c r="D156" s="67"/>
+      <c r="E156" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B157" s="72"/>
-      <c r="C157" s="70"/>
-      <c r="D157" s="70"/>
-      <c r="E157" s="69">
+      <c r="B157" s="68"/>
+      <c r="C157" s="67"/>
+      <c r="D157" s="67"/>
+      <c r="E157" s="63">
         <v>421892</v>
       </c>
     </row>
     <row r="158" spans="2:5" ht="15">
-      <c r="B158" s="72"/>
-      <c r="C158" s="70"/>
-      <c r="D158" s="70"/>
-      <c r="E158" s="69">
+      <c r="B158" s="68"/>
+      <c r="C158" s="67"/>
+      <c r="D158" s="67"/>
+      <c r="E158" s="63">
         <v>450407</v>
       </c>
     </row>
     <row r="159" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B159" s="72" t="s">
+      <c r="B159" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="C159" s="70" t="s">
+      <c r="C159" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D159" s="70" t="s">
+      <c r="D159" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="E159" s="69">
+      <c r="E159" s="63">
         <v>518841</v>
       </c>
     </row>
     <row r="160" spans="2:5" ht="15">
-      <c r="B160" s="72"/>
-      <c r="C160" s="70"/>
-      <c r="D160" s="70"/>
-      <c r="E160" s="69">
+      <c r="B160" s="68"/>
+      <c r="C160" s="67"/>
+      <c r="D160" s="67"/>
+      <c r="E160" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="161" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B161" s="72" t="s">
+      <c r="B161" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="C161" s="70" t="s">
+      <c r="C161" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D161" s="70" t="s">
+      <c r="D161" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="E161" s="69">
+      <c r="E161" s="63">
         <v>459419</v>
       </c>
     </row>
     <row r="162" spans="2:5" ht="15">
-      <c r="B162" s="72"/>
-      <c r="C162" s="70"/>
-      <c r="D162" s="70"/>
-      <c r="E162" s="69">
+      <c r="B162" s="68"/>
+      <c r="C162" s="67"/>
+      <c r="D162" s="67"/>
+      <c r="E162" s="63">
         <v>553643</v>
       </c>
     </row>
     <row r="163" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B163" s="72" t="s">
+      <c r="B163" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="C163" s="70" t="s">
+      <c r="C163" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="D163" s="70" t="s">
+      <c r="D163" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="E163" s="69">
+      <c r="E163" s="63">
         <v>518761</v>
       </c>
     </row>
     <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B164" s="72"/>
-      <c r="C164" s="70"/>
-      <c r="D164" s="70"/>
-      <c r="E164" s="69">
+      <c r="B164" s="68"/>
+      <c r="C164" s="67"/>
+      <c r="D164" s="67"/>
+      <c r="E164" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="165" spans="2:5" ht="15">
-      <c r="B165" s="72"/>
-      <c r="C165" s="70"/>
-      <c r="D165" s="70"/>
-      <c r="E165" s="69">
+      <c r="B165" s="68"/>
+      <c r="C165" s="67"/>
+      <c r="D165" s="67"/>
+      <c r="E165" s="63">
         <v>421892</v>
       </c>
     </row>
     <row r="166" spans="2:5" ht="15">
-      <c r="B166" s="71" t="s">
+      <c r="B166" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="C166" s="68" t="s">
+      <c r="C166" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D166" s="68" t="s">
+      <c r="D166" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="E166" s="69" t="s">
+      <c r="E166" s="63" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="167" spans="2:5" ht="15">
-      <c r="B167" s="71" t="s">
+      <c r="B167" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="C167" s="68" t="s">
+      <c r="C167" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D167" s="68" t="s">
+      <c r="D167" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="E167" s="69" t="s">
+      <c r="E167" s="63" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="27">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B133:B134"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B127:E127"/>
+    <mergeCell ref="B149:B151"/>
+    <mergeCell ref="C149:C151"/>
+    <mergeCell ref="D149:D151"/>
+    <mergeCell ref="B155:B158"/>
+    <mergeCell ref="C155:C158"/>
+    <mergeCell ref="D155:D158"/>
     <mergeCell ref="D163:D165"/>
     <mergeCell ref="C163:C165"/>
     <mergeCell ref="B163:B165"/>
@@ -2457,24 +2462,191 @@
     <mergeCell ref="B161:B162"/>
     <mergeCell ref="C161:C162"/>
     <mergeCell ref="D161:D162"/>
-    <mergeCell ref="B149:B151"/>
-    <mergeCell ref="C149:C151"/>
-    <mergeCell ref="D149:D151"/>
-    <mergeCell ref="B155:B158"/>
-    <mergeCell ref="C155:C158"/>
-    <mergeCell ref="D155:D158"/>
-    <mergeCell ref="B133:B134"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="D133:D134"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B127:E127"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B94:D94"/>
+  </mergeCells>
+  <phoneticPr fontId="54" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F6224-7F2A-BA4D-ABDF-DEDD326C8E0B}">
+  <dimension ref="B2:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="4.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="55" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="55" width="12.83203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="55" width="34.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="65"/>
+      <c r="C4" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="65"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="65"/>
+      <c r="C5" s="78" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="65"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15">
+      <c r="B7" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="65">
+        <v>0</v>
+      </c>
+      <c r="E7" s="79">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="80" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15">
+      <c r="B8" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="65">
+        <v>1000001</v>
+      </c>
+      <c r="E8" s="79">
+        <v>2000000</v>
+      </c>
+      <c r="F8" s="80" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15">
+      <c r="B9" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="65">
+        <v>2000001</v>
+      </c>
+      <c r="E9" s="79">
+        <v>3000000</v>
+      </c>
+      <c r="F9" s="80" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15">
+      <c r="B10" s="81" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="81">
+        <v>0</v>
+      </c>
+      <c r="E10" s="82">
+        <v>3000001</v>
+      </c>
+      <c r="F10" s="83">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15">
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15">
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="83">
+        <v>518761</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E10:E12"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new suggestCards Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A5136-7456-904A-B1C9-F823FC8D2808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A33679C-65A4-694E-948E-6F457C948FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="140">
   <si>
     <t>RETURN</t>
   </si>
@@ -377,12 +377,6 @@
     <t>Double max</t>
   </si>
   <si>
-    <t>Desde</t>
-  </si>
-  <si>
-    <t>Hasta</t>
-  </si>
-  <si>
     <t>Objeto</t>
   </si>
   <si>
@@ -392,18 +386,12 @@
     <t>C3</t>
   </si>
   <si>
-    <t>Rules String[] suggestCards3 (String situation, DoubleValue income)</t>
-  </si>
-  <si>
     <t>income &lt;= max</t>
   </si>
   <si>
     <t>min &lt;= income</t>
   </si>
   <si>
-    <t>sit = situation</t>
-  </si>
-  <si>
     <t>String sit</t>
   </si>
   <si>
@@ -413,9 +401,6 @@
     <t>R40</t>
   </si>
   <si>
-    <t>situation = sit</t>
-  </si>
-  <si>
     <t>Rules String[] suggestCards3 (String situation, Double income)</t>
   </si>
   <si>
@@ -426,6 +411,36 @@
   </si>
   <si>
     <t>IncomeOut</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>R80</t>
+  </si>
+  <si>
+    <t>R90</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>R110</t>
+  </si>
+  <si>
+    <t>R120</t>
+  </si>
+  <si>
+    <t>R130</t>
+  </si>
+  <si>
+    <t>Rules String[] suggestCards (String situation, Double income)</t>
   </si>
 </sst>
 </file>
@@ -433,7 +448,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="60">
+  <fonts count="61">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -745,8 +760,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -788,6 +809,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1100,52 +1127,57 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="58" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="59" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="58" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="58" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1488,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:E167"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E149" sqref="E149:E151"/>
+    <sheetView topLeftCell="A145" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152:C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1500,167 +1532,21 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4">
-      <c r="B4" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
+    <row r="4" spans="2:4"/>
+    <row r="5" spans="2:4"/>
+    <row r="6" spans="2:4"/>
+    <row r="7" spans="2:4"/>
+    <row r="8" spans="2:4"/>
+    <row r="9" spans="2:4"/>
+    <row r="10" spans="2:4"/>
+    <row r="11" spans="2:4"/>
+    <row r="12" spans="2:4"/>
+    <row r="13" spans="2:4"/>
+    <row r="14" spans="2:4"/>
+    <row r="15" spans="2:4"/>
+    <row r="16" spans="2:4"/>
+    <row r="17" spans="2:4"/>
+    <row r="18" spans="2:4"/>
     <row r="32" spans="2:4">
       <c r="B32" s="34" t="s">
         <v>24</v>
@@ -1686,10 +1572,10 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="73" t="s">
+      <c r="B60" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="73"/>
+      <c r="C60" s="70"/>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="35" t="s">
@@ -1708,10 +1594,10 @@
       </c>
     </row>
     <row r="68" spans="2:3">
-      <c r="B68" s="73" t="s">
+      <c r="B68" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C68" s="73"/>
+      <c r="C68" s="70"/>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="36" t="s">
@@ -1762,10 +1648,10 @@
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85" s="73" t="s">
+      <c r="B85" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="73"/>
+      <c r="C85" s="70"/>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" s="37" t="s">
@@ -1792,11 +1678,11 @@
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="B94" s="73" t="s">
+      <c r="B94" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C94" s="73"/>
-      <c r="D94" s="73"/>
+      <c r="C94" s="70"/>
+      <c r="D94" s="70"/>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" s="38" t="s">
@@ -1920,10 +1806,10 @@
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="71" t="s">
+      <c r="B107" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="71"/>
+      <c r="C107" s="69"/>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="39" t="s">
@@ -1990,10 +1876,10 @@
       </c>
     </row>
     <row r="117" spans="2:5">
-      <c r="B117" s="72" t="s">
+      <c r="B117" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C117" s="73"/>
+      <c r="C117" s="70"/>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="57" t="s">
@@ -2074,13 +1960,13 @@
       </c>
     </row>
     <row r="133" spans="2:5" s="55" customFormat="1" ht="18">
-      <c r="B133" s="69" t="s">
+      <c r="B133" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C133" s="69" t="s">
+      <c r="C133" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="D133" s="69">
+      <c r="D133" s="71">
         <v>1</v>
       </c>
       <c r="E133" s="59" t="s">
@@ -2088,9 +1974,9 @@
       </c>
     </row>
     <row r="134" spans="2:5" ht="18">
-      <c r="B134" s="69"/>
-      <c r="C134" s="69"/>
-      <c r="D134" s="69"/>
+      <c r="B134" s="71"/>
+      <c r="C134" s="71"/>
+      <c r="D134" s="71"/>
       <c r="E134" s="59" t="s">
         <v>103</v>
       </c>
@@ -2123,345 +2009,45 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="2:5" ht="15">
-      <c r="B141" s="70" t="s">
-        <v>114</v>
-      </c>
-      <c r="C141" s="70"/>
-      <c r="D141" s="70"/>
-      <c r="E141" s="70"/>
-    </row>
-    <row r="142" spans="2:5" ht="14">
-      <c r="B142" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="C142" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="D142" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="E142" s="60" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" ht="14">
-      <c r="B143" s="61"/>
-      <c r="C143" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="D143" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="E143" s="61"/>
-    </row>
-    <row r="144" spans="2:5" ht="14">
-      <c r="B144" s="61"/>
-      <c r="C144" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="D144" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="E144" s="61"/>
-    </row>
-    <row r="145" spans="2:5" ht="14">
-      <c r="B145" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C145" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="D145" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="E145" s="61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" ht="15">
-      <c r="B146" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="C146" s="66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D146" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="E146" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5" ht="15">
-      <c r="B147" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="C147" s="66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D147" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E147" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="148" spans="2:5" ht="15">
-      <c r="B148" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="C148" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D148" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E148" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B149" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="C149" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D149" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="E149" s="63">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B150" s="68"/>
-      <c r="C150" s="67"/>
-      <c r="D150" s="67"/>
-      <c r="E150" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" ht="15">
-      <c r="B151" s="68"/>
-      <c r="C151" s="67"/>
-      <c r="D151" s="67"/>
-      <c r="E151" s="63">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5" ht="15">
-      <c r="B152" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="C152" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="D152" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="E152" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="153" spans="2:5" ht="15">
-      <c r="B153" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="C153" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="D153" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E153" s="63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="154" spans="2:5" ht="15">
-      <c r="B154" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="C154" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="D154" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="E154" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="155" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B155" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="C155" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="D155" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="E155" s="63">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B156" s="68"/>
-      <c r="C156" s="67"/>
-      <c r="D156" s="67"/>
-      <c r="E156" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B157" s="68"/>
-      <c r="C157" s="67"/>
-      <c r="D157" s="67"/>
-      <c r="E157" s="63">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="158" spans="2:5" ht="15">
-      <c r="B158" s="68"/>
-      <c r="C158" s="67"/>
-      <c r="D158" s="67"/>
-      <c r="E158" s="63">
-        <v>450407</v>
-      </c>
-    </row>
-    <row r="159" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B159" s="68" t="s">
-        <v>108</v>
-      </c>
-      <c r="C159" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="D159" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="E159" s="63">
-        <v>518841</v>
-      </c>
-    </row>
-    <row r="160" spans="2:5" ht="15">
-      <c r="B160" s="68"/>
-      <c r="C160" s="67"/>
-      <c r="D160" s="67"/>
-      <c r="E160" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="161" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B161" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="C161" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="D161" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="E161" s="63">
-        <v>459419</v>
-      </c>
-    </row>
-    <row r="162" spans="2:5" ht="15">
-      <c r="B162" s="68"/>
-      <c r="C162" s="67"/>
-      <c r="D162" s="67"/>
-      <c r="E162" s="63">
-        <v>553643</v>
-      </c>
-    </row>
-    <row r="163" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B163" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="C163" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="D163" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="E163" s="63">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B164" s="68"/>
-      <c r="C164" s="67"/>
-      <c r="D164" s="67"/>
-      <c r="E164" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="165" spans="2:5" ht="15">
-      <c r="B165" s="68"/>
-      <c r="C165" s="67"/>
-      <c r="D165" s="67"/>
-      <c r="E165" s="63">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="166" spans="2:5" ht="15">
-      <c r="B166" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="C166" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="D166" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="E166" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="167" spans="2:5" ht="15">
-      <c r="B167" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="C167" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="D167" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="E167" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
+    <row r="141" spans="2:5" ht="15"/>
+    <row r="142" spans="2:5" ht="14"/>
+    <row r="143" spans="2:5" ht="14"/>
+    <row r="144" spans="2:5" ht="14"/>
+    <row r="145" spans="2:5" ht="14"/>
+    <row r="146" spans="2:5" ht="15"/>
+    <row r="147" spans="2:5" ht="15"/>
+    <row r="148" spans="2:5" ht="15"/>
+    <row r="149" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="150" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="151" spans="2:5" ht="15"/>
+    <row r="152" spans="2:5" ht="15"/>
+    <row r="153" spans="2:5" ht="15"/>
+    <row r="154" spans="2:5" ht="15"/>
+    <row r="155" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
+    <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
+    <row r="158" spans="2:5" ht="15"/>
+    <row r="159" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="160" spans="2:5" ht="15"/>
+    <row r="161" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="162" spans="2:5" ht="15"/>
+    <row r="163" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
+    <row r="165" spans="2:5" ht="15"/>
+    <row r="166" spans="2:5" ht="15"/>
+    <row r="167" spans="2:5" ht="15"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B133:B134"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B127:E127"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="B94:D94"/>
-    <mergeCell ref="B133:B134"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="D133:D134"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B127:E127"/>
-    <mergeCell ref="B149:B151"/>
-    <mergeCell ref="C149:C151"/>
-    <mergeCell ref="D149:D151"/>
-    <mergeCell ref="B155:B158"/>
-    <mergeCell ref="C155:C158"/>
-    <mergeCell ref="D155:D158"/>
-    <mergeCell ref="D163:D165"/>
-    <mergeCell ref="C163:C165"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="D159:D160"/>
-    <mergeCell ref="C159:C160"/>
-    <mergeCell ref="B159:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="D161:D162"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2470,24 +2056,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F6224-7F2A-BA4D-ABDF-DEDD326C8E0B}">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="4.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.5" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="55" width="12.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="55" width="12.83203125" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" style="55" width="17.33203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="55" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="77" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
@@ -2495,153 +2080,385 @@
       <c r="F2" s="77"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="75" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="65"/>
-      <c r="C4" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="78" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" s="78" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" s="65"/>
+      <c r="E4" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="68"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="65"/>
-      <c r="C5" s="78" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="68"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="F5" s="65"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="76" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>134</v>
-      </c>
-      <c r="F6" s="76" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15">
-      <c r="B7" s="65" t="s">
+      <c r="D6" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="78">
         <v>0</v>
       </c>
       <c r="E7" s="79">
         <v>1000000</v>
       </c>
-      <c r="F7" s="80" t="s">
+      <c r="F7" s="79" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15">
-      <c r="B8" s="65" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="84" t="s">
+    <row r="8" spans="2:6">
+      <c r="B8" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="78">
         <v>1000001</v>
       </c>
       <c r="E8" s="79">
         <v>2000000</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="79" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15">
-      <c r="B9" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="84" t="s">
+    <row r="9" spans="2:6">
+      <c r="B9" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="78">
         <v>2000001</v>
       </c>
       <c r="E9" s="79">
         <v>3000000</v>
       </c>
-      <c r="F9" s="80" t="s">
+      <c r="F9" s="79" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15">
-      <c r="B10" s="81" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="81" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" s="80" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="81">
+      <c r="D10" s="80">
+        <v>3000001</v>
+      </c>
+      <c r="E10" s="81">
+        <v>4500000</v>
+      </c>
+      <c r="F10" s="79">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="79">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="79">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="82" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="82">
         <v>0</v>
       </c>
-      <c r="E10" s="82">
-        <v>3000001</v>
-      </c>
-      <c r="F10" s="83">
+      <c r="E13" s="82">
+        <v>1000000</v>
+      </c>
+      <c r="F13" s="82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="82" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="82">
+        <v>1000001</v>
+      </c>
+      <c r="E14" s="82">
+        <v>10000000</v>
+      </c>
+      <c r="F14" s="82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="83" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="83">
+        <v>0</v>
+      </c>
+      <c r="E15" s="83">
+        <v>2000000</v>
+      </c>
+      <c r="F15" s="83" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="84">
+        <v>2000001</v>
+      </c>
+      <c r="E16" s="84">
+        <v>4000000</v>
+      </c>
+      <c r="F16" s="83">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="83">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="84"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="83">
         <v>421892</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15">
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="83">
+    <row r="19" spans="2:6">
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="83">
+        <v>450407</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="84" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="84">
+        <v>4000001</v>
+      </c>
+      <c r="E20" s="84">
+        <v>6000000</v>
+      </c>
+      <c r="F20" s="83">
+        <v>518841</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="83">
         <v>450408</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="15">
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="83">
+    <row r="22" spans="2:6">
+      <c r="B22" s="84" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="84">
+        <v>6000001</v>
+      </c>
+      <c r="E22" s="84">
+        <v>8000000</v>
+      </c>
+      <c r="F22" s="83">
+        <v>459419</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="83">
+        <v>553643</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="85">
+        <v>300000</v>
+      </c>
+      <c r="E24" s="85">
+        <v>10000000</v>
+      </c>
+      <c r="F24" s="82">
         <v>518761</v>
       </c>
     </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="85"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="82">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="82">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="82" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="82">
+        <v>0</v>
+      </c>
+      <c r="E27" s="82">
+        <v>2999999</v>
+      </c>
+      <c r="F27" s="82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="83">
+        <v>0</v>
+      </c>
+      <c r="E28" s="83">
+        <v>10000000</v>
+      </c>
+      <c r="F28" s="83" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="21">
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B10:B12"/>

</xml_diff>

<commit_message>
backup Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="139">
   <si>
     <t>RETURN</t>
   </si>
@@ -438,16 +438,12 @@
   </si>
   <si>
     <t>R130</t>
-  </si>
-  <si>
-    <t>Rules String[] suggestCards (String situation, Double income)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="61">
     <font>
       <sz val="10"/>
@@ -802,7 +798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -814,7 +810,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -955,7 +951,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1526,27 +1522,173 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="27.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4"/>
-    <row r="5" spans="2:4"/>
-    <row r="6" spans="2:4"/>
-    <row r="7" spans="2:4"/>
-    <row r="8" spans="2:4"/>
-    <row r="9" spans="2:4"/>
-    <row r="10" spans="2:4"/>
-    <row r="11" spans="2:4"/>
-    <row r="12" spans="2:4"/>
-    <row r="13" spans="2:4"/>
-    <row r="14" spans="2:4"/>
-    <row r="15" spans="2:4"/>
-    <row r="16" spans="2:4"/>
-    <row r="17" spans="2:4"/>
-    <row r="18" spans="2:4"/>
+    <row r="4" spans="2:4">
+      <c r="B4" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="32" spans="2:4">
       <c r="B32" s="34" t="s">
         <v>24</v>
@@ -2009,41 +2151,341 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="2:5" ht="15"/>
-    <row r="142" spans="2:5" ht="14"/>
-    <row r="143" spans="2:5" ht="14"/>
-    <row r="144" spans="2:5" ht="14"/>
-    <row r="145" spans="2:5" ht="14"/>
-    <row r="146" spans="2:5" ht="15"/>
-    <row r="147" spans="2:5" ht="15"/>
-    <row r="148" spans="2:5" ht="15"/>
-    <row r="149" spans="2:5" s="55" customFormat="1" ht="15"/>
-    <row r="150" spans="2:5" s="55" customFormat="1" ht="15"/>
-    <row r="151" spans="2:5" ht="15"/>
-    <row r="152" spans="2:5" ht="15"/>
-    <row r="153" spans="2:5" ht="15"/>
-    <row r="154" spans="2:5" ht="15"/>
-    <row r="155" spans="2:5" s="55" customFormat="1" ht="15"/>
-    <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
-    <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
-    <row r="158" spans="2:5" ht="15"/>
-    <row r="159" spans="2:5" s="55" customFormat="1" ht="15"/>
-    <row r="160" spans="2:5" ht="15"/>
-    <row r="161" spans="2:5" s="55" customFormat="1" ht="15"/>
-    <row r="162" spans="2:5" ht="15"/>
-    <row r="163" spans="2:5" s="55" customFormat="1" ht="15"/>
-    <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
-    <row r="165" spans="2:5" ht="15"/>
-    <row r="166" spans="2:5" ht="15"/>
-    <row r="167" spans="2:5" ht="15"/>
+    <row r="141" spans="2:5" ht="15">
+      <c r="B141" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="C141" s="72"/>
+      <c r="D141" s="72"/>
+      <c r="E141" s="72"/>
+    </row>
+    <row r="142" spans="2:5" ht="14">
+      <c r="B142" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="C142" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="D142" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E142" s="60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" ht="14">
+      <c r="B143" s="61"/>
+      <c r="C143" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="D143" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E143" s="61"/>
+    </row>
+    <row r="144" spans="2:5" ht="14">
+      <c r="B144" s="61"/>
+      <c r="C144" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D144" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="E144" s="61"/>
+    </row>
+    <row r="145" spans="2:5" ht="14">
+      <c r="B145" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C145" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="D145" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E145" s="61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" ht="15">
+      <c r="B146" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="C146" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E146" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" ht="15">
+      <c r="B147" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="C147" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D147" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" ht="15">
+      <c r="B148" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C148" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D148" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E148" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" s="55" customFormat="1" ht="15">
+      <c r="B149" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="C149" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D149" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" s="63">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" s="55" customFormat="1" ht="15">
+      <c r="B150" s="75"/>
+      <c r="C150" s="76"/>
+      <c r="D150" s="76"/>
+      <c r="E150" s="63">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" ht="15">
+      <c r="B151" s="75"/>
+      <c r="C151" s="76"/>
+      <c r="D151" s="76"/>
+      <c r="E151" s="63">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="15">
+      <c r="B152" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="C152" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D152" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E152" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" ht="15">
+      <c r="B153" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="C153" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D153" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E153" s="63" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" ht="15">
+      <c r="B154" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C154" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D154" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E154" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" s="55" customFormat="1" ht="15">
+      <c r="B155" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="C155" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="E155" s="63">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
+      <c r="B156" s="75"/>
+      <c r="C156" s="76"/>
+      <c r="D156" s="76"/>
+      <c r="E156" s="63">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
+      <c r="B157" s="75"/>
+      <c r="C157" s="76"/>
+      <c r="D157" s="76"/>
+      <c r="E157" s="63">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5" ht="15">
+      <c r="B158" s="75"/>
+      <c r="C158" s="76"/>
+      <c r="D158" s="76"/>
+      <c r="E158" s="63">
+        <v>450407</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" s="55" customFormat="1" ht="15">
+      <c r="B159" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="C159" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D159" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E159" s="63">
+        <v>518841</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" ht="15">
+      <c r="B160" s="75"/>
+      <c r="C160" s="76"/>
+      <c r="D160" s="76"/>
+      <c r="E160" s="63">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" s="55" customFormat="1" ht="15">
+      <c r="B161" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="C161" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D161" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E161" s="63">
+        <v>459419</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" ht="15">
+      <c r="B162" s="75"/>
+      <c r="C162" s="76"/>
+      <c r="D162" s="76"/>
+      <c r="E162" s="63">
+        <v>553643</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" s="55" customFormat="1" ht="15">
+      <c r="B163" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="C163" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="D163" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="E163" s="63">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
+      <c r="B164" s="75"/>
+      <c r="C164" s="76"/>
+      <c r="D164" s="76"/>
+      <c r="E164" s="63">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" ht="15">
+      <c r="B165" s="75"/>
+      <c r="C165" s="76"/>
+      <c r="D165" s="76"/>
+      <c r="E165" s="63">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" ht="15">
+      <c r="B166" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C166" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D166" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" ht="15">
+      <c r="B167" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="C167" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="D167" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="E167" s="63" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D163:D165"/>
+    <mergeCell ref="C163:C165"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="D159:D160"/>
+    <mergeCell ref="C159:C160"/>
+    <mergeCell ref="B159:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="C161:C162"/>
+    <mergeCell ref="D161:D162"/>
+    <mergeCell ref="B149:B151"/>
+    <mergeCell ref="C149:C151"/>
+    <mergeCell ref="D149:D151"/>
+    <mergeCell ref="B155:B158"/>
+    <mergeCell ref="C155:C158"/>
+    <mergeCell ref="D155:D158"/>
     <mergeCell ref="B133:B134"/>
     <mergeCell ref="C133:C134"/>
     <mergeCell ref="D133:D134"/>
+    <mergeCell ref="B141:E141"/>
     <mergeCell ref="B107:C107"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="B127:E127"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B85:C85"/>
@@ -2064,15 +2506,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.5" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" style="55" width="17.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="55" width="34.0" collapsed="true"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="17.33203125" style="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34" style="55" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="77" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>

</xml_diff>

<commit_message>
backup old Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A33679C-65A4-694E-948E-6F457C948FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6043F773-9AE3-3946-ABE0-1CA3A074F910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
   <si>
     <t>RETURN</t>
   </si>
@@ -366,85 +365,13 @@
   </si>
   <si>
     <t>Rules String[] suggestCards2(String situation, DoubleRange income)</t>
-  </si>
-  <si>
-    <t>RET1</t>
-  </si>
-  <si>
-    <t>Double min</t>
-  </si>
-  <si>
-    <t>Double max</t>
-  </si>
-  <si>
-    <t>Objeto</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>income &lt;= max</t>
-  </si>
-  <si>
-    <t>min &lt;= income</t>
-  </si>
-  <si>
-    <t>String sit</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>Rules String[] suggestCards3 (String situation, Double income)</t>
-  </si>
-  <si>
-    <t>Situation</t>
-  </si>
-  <si>
-    <t>IncomeIni</t>
-  </si>
-  <si>
-    <t>IncomeOut</t>
-  </si>
-  <si>
-    <t>R50</t>
-  </si>
-  <si>
-    <t>R60</t>
-  </si>
-  <si>
-    <t>R70</t>
-  </si>
-  <si>
-    <t>R80</t>
-  </si>
-  <si>
-    <t>R90</t>
-  </si>
-  <si>
-    <t>R100</t>
-  </si>
-  <si>
-    <t>R110</t>
-  </si>
-  <si>
-    <t>R120</t>
-  </si>
-  <si>
-    <t>R130</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="61">
+  <fonts count="59">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -750,20 +677,8 @@
       <color indexed="8"/>
       <name val="&quot;Franklin Gothik Book&quot;"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,26 +711,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -921,21 +818,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="0"/>
       </left>
       <right style="thin">
@@ -953,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1123,12 +1005,9 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1148,33 +1027,6 @@
     </xf>
     <xf numFmtId="0" fontId="58" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1516,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:E167"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152:C167"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1529,11 +1381,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
@@ -1714,10 +1566,10 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="70" t="s">
+      <c r="B60" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="70"/>
+      <c r="C60" s="67"/>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="35" t="s">
@@ -1736,10 +1588,10 @@
       </c>
     </row>
     <row r="68" spans="2:3">
-      <c r="B68" s="70" t="s">
+      <c r="B68" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C68" s="70"/>
+      <c r="C68" s="67"/>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="36" t="s">
@@ -1790,10 +1642,10 @@
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85" s="70" t="s">
+      <c r="B85" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="70"/>
+      <c r="C85" s="67"/>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" s="37" t="s">
@@ -1820,11 +1672,11 @@
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="B94" s="70" t="s">
+      <c r="B94" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C94" s="70"/>
-      <c r="D94" s="70"/>
+      <c r="C94" s="67"/>
+      <c r="D94" s="67"/>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" s="38" t="s">
@@ -1948,10 +1800,10 @@
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="69" t="s">
+      <c r="B107" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="69"/>
+      <c r="C107" s="66"/>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="39" t="s">
@@ -2018,10 +1870,10 @@
       </c>
     </row>
     <row r="117" spans="2:5">
-      <c r="B117" s="73" t="s">
+      <c r="B117" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="C117" s="70"/>
+      <c r="C117" s="67"/>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="57" t="s">
@@ -2032,12 +1884,12 @@
       </c>
     </row>
     <row r="127" spans="2:5">
-      <c r="B127" s="74" t="s">
+      <c r="B127" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="C127" s="74"/>
-      <c r="D127" s="74"/>
-      <c r="E127" s="74"/>
+      <c r="C127" s="71"/>
+      <c r="D127" s="71"/>
+      <c r="E127" s="71"/>
     </row>
     <row r="128" spans="2:5" ht="18">
       <c r="B128" s="58" t="s">
@@ -2102,13 +1954,13 @@
       </c>
     </row>
     <row r="133" spans="2:5" s="55" customFormat="1" ht="18">
-      <c r="B133" s="71" t="s">
+      <c r="B133" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C133" s="71" t="s">
+      <c r="C133" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="D133" s="71">
+      <c r="D133" s="68">
         <v>1</v>
       </c>
       <c r="E133" s="59" t="s">
@@ -2116,9 +1968,9 @@
       </c>
     </row>
     <row r="134" spans="2:5" ht="18">
-      <c r="B134" s="71"/>
-      <c r="C134" s="71"/>
-      <c r="D134" s="71"/>
+      <c r="B134" s="68"/>
+      <c r="C134" s="68"/>
+      <c r="D134" s="68"/>
       <c r="E134" s="59" t="s">
         <v>103</v>
       </c>
@@ -2152,12 +2004,12 @@
       </c>
     </row>
     <row r="141" spans="2:5" ht="15">
-      <c r="B141" s="72" t="s">
+      <c r="B141" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="C141" s="72"/>
-      <c r="D141" s="72"/>
-      <c r="E141" s="72"/>
+      <c r="C141" s="69"/>
+      <c r="D141" s="69"/>
+      <c r="E141" s="69"/>
     </row>
     <row r="142" spans="2:5" ht="14">
       <c r="B142" s="60" t="s">
@@ -2250,13 +2102,13 @@
       </c>
     </row>
     <row r="149" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B149" s="75" t="s">
+      <c r="B149" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="C149" s="76" t="s">
+      <c r="C149" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D149" s="76" t="s">
+      <c r="D149" s="73" t="s">
         <v>8</v>
       </c>
       <c r="E149" s="63">
@@ -2264,17 +2116,17 @@
       </c>
     </row>
     <row r="150" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B150" s="75"/>
-      <c r="C150" s="76"/>
-      <c r="D150" s="76"/>
+      <c r="B150" s="72"/>
+      <c r="C150" s="73"/>
+      <c r="D150" s="73"/>
       <c r="E150" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="151" spans="2:5" ht="15">
-      <c r="B151" s="75"/>
-      <c r="C151" s="76"/>
-      <c r="D151" s="76"/>
+      <c r="B151" s="72"/>
+      <c r="C151" s="73"/>
+      <c r="D151" s="73"/>
       <c r="E151" s="63">
         <v>518761</v>
       </c>
@@ -2322,13 +2174,13 @@
       </c>
     </row>
     <row r="155" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B155" s="75" t="s">
+      <c r="B155" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="C155" s="76" t="s">
+      <c r="C155" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D155" s="76" t="s">
+      <c r="D155" s="73" t="s">
         <v>14</v>
       </c>
       <c r="E155" s="63">
@@ -2336,37 +2188,37 @@
       </c>
     </row>
     <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B156" s="75"/>
-      <c r="C156" s="76"/>
-      <c r="D156" s="76"/>
+      <c r="B156" s="72"/>
+      <c r="C156" s="73"/>
+      <c r="D156" s="73"/>
       <c r="E156" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B157" s="75"/>
-      <c r="C157" s="76"/>
-      <c r="D157" s="76"/>
+      <c r="B157" s="72"/>
+      <c r="C157" s="73"/>
+      <c r="D157" s="73"/>
       <c r="E157" s="63">
         <v>421892</v>
       </c>
     </row>
     <row r="158" spans="2:5" ht="15">
-      <c r="B158" s="75"/>
-      <c r="C158" s="76"/>
-      <c r="D158" s="76"/>
+      <c r="B158" s="72"/>
+      <c r="C158" s="73"/>
+      <c r="D158" s="73"/>
       <c r="E158" s="63">
         <v>450407</v>
       </c>
     </row>
     <row r="159" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B159" s="75" t="s">
+      <c r="B159" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C159" s="76" t="s">
+      <c r="C159" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D159" s="76" t="s">
+      <c r="D159" s="73" t="s">
         <v>15</v>
       </c>
       <c r="E159" s="63">
@@ -2374,21 +2226,21 @@
       </c>
     </row>
     <row r="160" spans="2:5" ht="15">
-      <c r="B160" s="75"/>
-      <c r="C160" s="76"/>
-      <c r="D160" s="76"/>
+      <c r="B160" s="72"/>
+      <c r="C160" s="73"/>
+      <c r="D160" s="73"/>
       <c r="E160" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="161" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B161" s="75" t="s">
+      <c r="B161" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="C161" s="76" t="s">
+      <c r="C161" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D161" s="76" t="s">
+      <c r="D161" s="73" t="s">
         <v>16</v>
       </c>
       <c r="E161" s="63">
@@ -2396,21 +2248,21 @@
       </c>
     </row>
     <row r="162" spans="2:5" ht="15">
-      <c r="B162" s="75"/>
-      <c r="C162" s="76"/>
-      <c r="D162" s="76"/>
+      <c r="B162" s="72"/>
+      <c r="C162" s="73"/>
+      <c r="D162" s="73"/>
       <c r="E162" s="63">
         <v>553643</v>
       </c>
     </row>
     <row r="163" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B163" s="75" t="s">
+      <c r="B163" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="C163" s="76" t="s">
+      <c r="C163" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="D163" s="76" t="s">
+      <c r="D163" s="73" t="s">
         <v>19</v>
       </c>
       <c r="E163" s="63">
@@ -2418,17 +2270,17 @@
       </c>
     </row>
     <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B164" s="75"/>
-      <c r="C164" s="76"/>
-      <c r="D164" s="76"/>
+      <c r="B164" s="72"/>
+      <c r="C164" s="73"/>
+      <c r="D164" s="73"/>
       <c r="E164" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="165" spans="2:5" ht="15">
-      <c r="B165" s="75"/>
-      <c r="C165" s="76"/>
-      <c r="D165" s="76"/>
+      <c r="B165" s="72"/>
+      <c r="C165" s="73"/>
+      <c r="D165" s="73"/>
       <c r="E165" s="63">
         <v>421892</v>
       </c>
@@ -2494,420 +2346,4 @@
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F6224-7F2A-BA4D-ABDF-DEDD326C8E0B}">
-  <dimension ref="B2:F28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="17.33203125" style="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34" style="55" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6">
-      <c r="B2" s="77" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="66" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="66" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="68"/>
-      <c r="C4" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>121</v>
-      </c>
-      <c r="F4" s="68"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="68"/>
-      <c r="C5" s="68" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="68" t="s">
-        <v>117</v>
-      </c>
-      <c r="F5" s="68"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="67" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" s="67" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="78">
-        <v>0</v>
-      </c>
-      <c r="E7" s="79">
-        <v>1000000</v>
-      </c>
-      <c r="F7" s="79" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="78">
-        <v>1000001</v>
-      </c>
-      <c r="E8" s="79">
-        <v>2000000</v>
-      </c>
-      <c r="F8" s="79" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="78" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="78">
-        <v>2000001</v>
-      </c>
-      <c r="E9" s="79">
-        <v>3000000</v>
-      </c>
-      <c r="F9" s="79" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="80" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="80">
-        <v>3000001</v>
-      </c>
-      <c r="E10" s="81">
-        <v>4500000</v>
-      </c>
-      <c r="F10" s="79">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="79">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="79">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="82" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="82">
-        <v>0</v>
-      </c>
-      <c r="E13" s="82">
-        <v>1000000</v>
-      </c>
-      <c r="F13" s="82" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="82" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="82">
-        <v>1000001</v>
-      </c>
-      <c r="E14" s="82">
-        <v>10000000</v>
-      </c>
-      <c r="F14" s="82" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="83" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="83" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="83">
-        <v>0</v>
-      </c>
-      <c r="E15" s="83">
-        <v>2000000</v>
-      </c>
-      <c r="F15" s="83" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="84" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="84" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="84">
-        <v>2000001</v>
-      </c>
-      <c r="E16" s="84">
-        <v>4000000</v>
-      </c>
-      <c r="F16" s="83">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="83">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="83">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="83">
-        <v>450407</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="84" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="84" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="84">
-        <v>4000001</v>
-      </c>
-      <c r="E20" s="84">
-        <v>6000000</v>
-      </c>
-      <c r="F20" s="83">
-        <v>518841</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="83">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="84" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="84" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="84">
-        <v>6000001</v>
-      </c>
-      <c r="E22" s="84">
-        <v>8000000</v>
-      </c>
-      <c r="F22" s="83">
-        <v>459419</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="83">
-        <v>553643</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="85">
-        <v>300000</v>
-      </c>
-      <c r="E24" s="85">
-        <v>10000000</v>
-      </c>
-      <c r="F24" s="82">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="82">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="85"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="82">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="82" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="82" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="82">
-        <v>0</v>
-      </c>
-      <c r="E27" s="82">
-        <v>2999999</v>
-      </c>
-      <c r="F27" s="82" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="83" t="s">
-        <v>138</v>
-      </c>
-      <c r="C28" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="83">
-        <v>0</v>
-      </c>
-      <c r="E28" s="83">
-        <v>10000000</v>
-      </c>
-      <c r="F28" s="83" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E10:E12"/>
-  </mergeCells>
-  <phoneticPr fontId="54" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
restore backup Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6043F773-9AE3-3946-ABE0-1CA3A074F910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A33679C-65A4-694E-948E-6F457C948FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="139">
   <si>
     <t>RETURN</t>
   </si>
@@ -365,13 +366,86 @@
   </si>
   <si>
     <t>Rules String[] suggestCards2(String situation, DoubleRange income)</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>Double min</t>
+  </si>
+  <si>
+    <t>Double max</t>
+  </si>
+  <si>
+    <t>Objeto</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>income &lt;= max</t>
+  </si>
+  <si>
+    <t>min &lt;= income</t>
+  </si>
+  <si>
+    <t>String sit</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>Rules String[] suggestCards3 (String situation, Double income)</t>
+  </si>
+  <si>
+    <t>Situation</t>
+  </si>
+  <si>
+    <t>IncomeIni</t>
+  </si>
+  <si>
+    <t>IncomeOut</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>R80</t>
+  </si>
+  <si>
+    <t>R90</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>R110</t>
+  </si>
+  <si>
+    <t>R120</t>
+  </si>
+  <si>
+    <t>R130</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="59">
+  <numFmts count="0"/>
+  <fonts count="61">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -677,8 +751,20 @@
       <color indexed="8"/>
       <name val="&quot;Franklin Gothik Book&quot;"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -711,8 +797,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -818,6 +922,21 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="0"/>
       </left>
       <right style="thin">
@@ -835,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1005,9 +1124,12 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,6 +1149,33 @@
     </xf>
     <xf numFmtId="0" fontId="58" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1368,24 +1517,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView topLeftCell="A145" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152:C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
@@ -1566,10 +1715,10 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="67" t="s">
+      <c r="B60" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="67"/>
+      <c r="C60" s="70"/>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="35" t="s">
@@ -1588,10 +1737,10 @@
       </c>
     </row>
     <row r="68" spans="2:3">
-      <c r="B68" s="67" t="s">
+      <c r="B68" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C68" s="67"/>
+      <c r="C68" s="70"/>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="36" t="s">
@@ -1642,10 +1791,10 @@
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85" s="67" t="s">
+      <c r="B85" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="67"/>
+      <c r="C85" s="70"/>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" s="37" t="s">
@@ -1672,11 +1821,11 @@
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="B94" s="67" t="s">
+      <c r="B94" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C94" s="67"/>
-      <c r="D94" s="67"/>
+      <c r="C94" s="70"/>
+      <c r="D94" s="70"/>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" s="38" t="s">
@@ -1800,10 +1949,10 @@
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="66" t="s">
+      <c r="B107" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="66"/>
+      <c r="C107" s="69"/>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="39" t="s">
@@ -1869,147 +2018,25 @@
         <v>76</v>
       </c>
     </row>
-    <row r="117" spans="2:5">
-      <c r="B117" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="C117" s="67"/>
-    </row>
-    <row r="118" spans="2:5">
-      <c r="B118" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="C118" s="56" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5">
-      <c r="B127" s="71" t="s">
-        <v>101</v>
-      </c>
-      <c r="C127" s="71"/>
-      <c r="D127" s="71"/>
-      <c r="E127" s="71"/>
-    </row>
-    <row r="128" spans="2:5" ht="18">
-      <c r="B128" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="C128" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="D128" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="E128" s="58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" ht="18">
-      <c r="B129" s="59"/>
-      <c r="C129" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="D129" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="E129" s="59"/>
-    </row>
-    <row r="130" spans="2:5" ht="18">
-      <c r="B130" s="59"/>
-      <c r="C130" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="D130" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="E130" s="59"/>
-    </row>
-    <row r="131" spans="2:5" ht="18">
-      <c r="B131" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="C131" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="D131" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="E131" s="59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="132" spans="2:5" ht="18">
-      <c r="B132" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="C132" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="D132" s="59">
-        <v>1</v>
-      </c>
-      <c r="E132" s="59" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" s="55" customFormat="1" ht="18">
-      <c r="B133" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="C133" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="D133" s="68">
-        <v>1</v>
-      </c>
-      <c r="E133" s="59" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" ht="18">
-      <c r="B134" s="68"/>
-      <c r="C134" s="68"/>
-      <c r="D134" s="68"/>
-      <c r="E134" s="59" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" ht="18">
-      <c r="B135" s="59" t="s">
-        <v>97</v>
-      </c>
-      <c r="C135" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="D135" s="59">
-        <v>1</v>
-      </c>
-      <c r="E135" s="59" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" ht="18">
-      <c r="B136" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="C136" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="D136" s="59">
-        <v>1</v>
-      </c>
-      <c r="E136" s="59" t="s">
-        <v>100</v>
-      </c>
-    </row>
+    <row r="117" spans="2:5"/>
+    <row r="118" spans="2:5"/>
+    <row r="127" spans="2:5"/>
+    <row r="128" spans="2:5" ht="18"/>
+    <row r="129" spans="2:5" ht="18"/>
+    <row r="130" spans="2:5" ht="18"/>
+    <row r="131" spans="2:5" ht="18"/>
+    <row r="132" spans="2:5" ht="18"/>
+    <row r="133" spans="2:5" s="55" customFormat="1" ht="18"/>
+    <row r="134" spans="2:5" ht="18"/>
+    <row r="135" spans="2:5" ht="18"/>
+    <row r="136" spans="2:5" ht="18"/>
     <row r="141" spans="2:5" ht="15">
-      <c r="B141" s="69" t="s">
+      <c r="B141" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="C141" s="69"/>
-      <c r="D141" s="69"/>
-      <c r="E141" s="69"/>
+      <c r="C141" s="72"/>
+      <c r="D141" s="72"/>
+      <c r="E141" s="72"/>
     </row>
     <row r="142" spans="2:5" ht="14">
       <c r="B142" s="60" t="s">
@@ -2102,13 +2129,13 @@
       </c>
     </row>
     <row r="149" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B149" s="72" t="s">
+      <c r="B149" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="C149" s="73" t="s">
+      <c r="C149" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="D149" s="73" t="s">
+      <c r="D149" s="76" t="s">
         <v>8</v>
       </c>
       <c r="E149" s="63">
@@ -2116,17 +2143,17 @@
       </c>
     </row>
     <row r="150" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B150" s="72"/>
-      <c r="C150" s="73"/>
-      <c r="D150" s="73"/>
+      <c r="B150" s="75"/>
+      <c r="C150" s="76"/>
+      <c r="D150" s="76"/>
       <c r="E150" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="151" spans="2:5" ht="15">
-      <c r="B151" s="72"/>
-      <c r="C151" s="73"/>
-      <c r="D151" s="73"/>
+      <c r="B151" s="75"/>
+      <c r="C151" s="76"/>
+      <c r="D151" s="76"/>
       <c r="E151" s="63">
         <v>518761</v>
       </c>
@@ -2174,13 +2201,13 @@
       </c>
     </row>
     <row r="155" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B155" s="72" t="s">
+      <c r="B155" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="C155" s="73" t="s">
+      <c r="C155" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D155" s="73" t="s">
+      <c r="D155" s="76" t="s">
         <v>14</v>
       </c>
       <c r="E155" s="63">
@@ -2188,37 +2215,37 @@
       </c>
     </row>
     <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B156" s="72"/>
-      <c r="C156" s="73"/>
-      <c r="D156" s="73"/>
+      <c r="B156" s="75"/>
+      <c r="C156" s="76"/>
+      <c r="D156" s="76"/>
       <c r="E156" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B157" s="72"/>
-      <c r="C157" s="73"/>
-      <c r="D157" s="73"/>
+      <c r="B157" s="75"/>
+      <c r="C157" s="76"/>
+      <c r="D157" s="76"/>
       <c r="E157" s="63">
         <v>421892</v>
       </c>
     </row>
     <row r="158" spans="2:5" ht="15">
-      <c r="B158" s="72"/>
-      <c r="C158" s="73"/>
-      <c r="D158" s="73"/>
+      <c r="B158" s="75"/>
+      <c r="C158" s="76"/>
+      <c r="D158" s="76"/>
       <c r="E158" s="63">
         <v>450407</v>
       </c>
     </row>
     <row r="159" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B159" s="72" t="s">
+      <c r="B159" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="C159" s="73" t="s">
+      <c r="C159" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D159" s="73" t="s">
+      <c r="D159" s="76" t="s">
         <v>15</v>
       </c>
       <c r="E159" s="63">
@@ -2226,21 +2253,21 @@
       </c>
     </row>
     <row r="160" spans="2:5" ht="15">
-      <c r="B160" s="72"/>
-      <c r="C160" s="73"/>
-      <c r="D160" s="73"/>
+      <c r="B160" s="75"/>
+      <c r="C160" s="76"/>
+      <c r="D160" s="76"/>
       <c r="E160" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="161" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B161" s="72" t="s">
+      <c r="B161" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="C161" s="73" t="s">
+      <c r="C161" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D161" s="73" t="s">
+      <c r="D161" s="76" t="s">
         <v>16</v>
       </c>
       <c r="E161" s="63">
@@ -2248,21 +2275,21 @@
       </c>
     </row>
     <row r="162" spans="2:5" ht="15">
-      <c r="B162" s="72"/>
-      <c r="C162" s="73"/>
-      <c r="D162" s="73"/>
+      <c r="B162" s="75"/>
+      <c r="C162" s="76"/>
+      <c r="D162" s="76"/>
       <c r="E162" s="63">
         <v>553643</v>
       </c>
     </row>
     <row r="163" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B163" s="72" t="s">
+      <c r="B163" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="C163" s="73" t="s">
+      <c r="C163" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="D163" s="73" t="s">
+      <c r="D163" s="76" t="s">
         <v>19</v>
       </c>
       <c r="E163" s="63">
@@ -2270,17 +2297,17 @@
       </c>
     </row>
     <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B164" s="72"/>
-      <c r="C164" s="73"/>
-      <c r="D164" s="73"/>
+      <c r="B164" s="75"/>
+      <c r="C164" s="76"/>
+      <c r="D164" s="76"/>
       <c r="E164" s="63">
         <v>450408</v>
       </c>
     </row>
     <row r="165" spans="2:5" ht="15">
-      <c r="B165" s="72"/>
-      <c r="C165" s="73"/>
-      <c r="D165" s="73"/>
+      <c r="B165" s="75"/>
+      <c r="C165" s="76"/>
+      <c r="D165" s="76"/>
       <c r="E165" s="63">
         <v>421892</v>
       </c>
@@ -2330,13 +2357,8 @@
     <mergeCell ref="B155:B158"/>
     <mergeCell ref="C155:C158"/>
     <mergeCell ref="D155:D158"/>
-    <mergeCell ref="B133:B134"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="D133:D134"/>
     <mergeCell ref="B141:E141"/>
     <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B127:E127"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B68:C68"/>
@@ -2346,4 +2368,420 @@
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F6224-7F2A-BA4D-ABDF-DEDD326C8E0B}">
+  <dimension ref="B2:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" style="55" width="17.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="55" width="34.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="68"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="68"/>
+      <c r="C5" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="68"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="78">
+        <v>0</v>
+      </c>
+      <c r="E7" s="79">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="78">
+        <v>1000001</v>
+      </c>
+      <c r="E8" s="79">
+        <v>2000000</v>
+      </c>
+      <c r="F8" s="79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="78">
+        <v>2000001</v>
+      </c>
+      <c r="E9" s="79">
+        <v>3000000</v>
+      </c>
+      <c r="F9" s="79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="80" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="80">
+        <v>3000001</v>
+      </c>
+      <c r="E10" s="81">
+        <v>4500000</v>
+      </c>
+      <c r="F10" s="79">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="79">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="79">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="82" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="82">
+        <v>0</v>
+      </c>
+      <c r="E13" s="82">
+        <v>1000000</v>
+      </c>
+      <c r="F13" s="82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="82" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="82">
+        <v>1000001</v>
+      </c>
+      <c r="E14" s="82">
+        <v>10000000</v>
+      </c>
+      <c r="F14" s="82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="83" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="83">
+        <v>0</v>
+      </c>
+      <c r="E15" s="83">
+        <v>2000000</v>
+      </c>
+      <c r="F15" s="83" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="84">
+        <v>2000001</v>
+      </c>
+      <c r="E16" s="84">
+        <v>4000000</v>
+      </c>
+      <c r="F16" s="83">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="83">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="84"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="83">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="83">
+        <v>450407</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="84" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="84">
+        <v>4000001</v>
+      </c>
+      <c r="E20" s="84">
+        <v>6000000</v>
+      </c>
+      <c r="F20" s="83">
+        <v>518841</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="83">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="84" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="84">
+        <v>6000001</v>
+      </c>
+      <c r="E22" s="84">
+        <v>8000000</v>
+      </c>
+      <c r="F22" s="83">
+        <v>459419</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="83">
+        <v>553643</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="85">
+        <v>300000</v>
+      </c>
+      <c r="E24" s="85">
+        <v>10000000</v>
+      </c>
+      <c r="F24" s="82">
+        <v>518761</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="85"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="82">
+        <v>450408</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="82">
+        <v>421892</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="82" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="82">
+        <v>0</v>
+      </c>
+      <c r="E27" s="82">
+        <v>2999999</v>
+      </c>
+      <c r="F27" s="82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="83">
+        <v>0</v>
+      </c>
+      <c r="E28" s="83">
+        <v>10000000</v>
+      </c>
+      <c r="F28" s="83" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E10:E12"/>
+  </mergeCells>
+  <phoneticPr fontId="54" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
suggestCards OK Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="140">
   <si>
     <t>RETURN</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>R130</t>
+  </si>
+  <si>
+    <t>Rules String[] suggestCards (String situation, Double income)</t>
   </si>
 </sst>
 </file>
@@ -799,7 +802,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -811,7 +814,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -952,7 +955,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1515,7 +1518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:E167"/>
+  <dimension ref="B4:D167"/>
   <sheetViews>
     <sheetView topLeftCell="A145" zoomScale="125" workbookViewId="0">
       <selection activeCell="C152" sqref="C152:C167"/>
@@ -1529,167 +1532,21 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4">
-      <c r="B4" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
+    <row r="4" spans="2:4"/>
+    <row r="5" spans="2:4"/>
+    <row r="6" spans="2:4"/>
+    <row r="7" spans="2:4"/>
+    <row r="8" spans="2:4"/>
+    <row r="9" spans="2:4"/>
+    <row r="10" spans="2:4"/>
+    <row r="11" spans="2:4"/>
+    <row r="12" spans="2:4"/>
+    <row r="13" spans="2:4"/>
+    <row r="14" spans="2:4"/>
+    <row r="15" spans="2:4"/>
+    <row r="16" spans="2:4"/>
+    <row r="17" spans="2:4"/>
+    <row r="18" spans="2:4"/>
     <row r="32" spans="2:4">
       <c r="B32" s="34" t="s">
         <v>24</v>
@@ -2030,336 +1887,36 @@
     <row r="134" spans="2:5" ht="18"/>
     <row r="135" spans="2:5" ht="18"/>
     <row r="136" spans="2:5" ht="18"/>
-    <row r="141" spans="2:5" ht="15">
-      <c r="B141" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="C141" s="72"/>
-      <c r="D141" s="72"/>
-      <c r="E141" s="72"/>
-    </row>
-    <row r="142" spans="2:5" ht="14">
-      <c r="B142" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="C142" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="D142" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="E142" s="60" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" ht="14">
-      <c r="B143" s="61"/>
-      <c r="C143" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="D143" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="E143" s="61"/>
-    </row>
-    <row r="144" spans="2:5" ht="14">
-      <c r="B144" s="61"/>
-      <c r="C144" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="D144" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="E144" s="61"/>
-    </row>
-    <row r="145" spans="2:5" ht="14">
-      <c r="B145" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C145" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="D145" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="E145" s="61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" ht="15">
-      <c r="B146" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="C146" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D146" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="E146" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5" ht="15">
-      <c r="B147" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="C147" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D147" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E147" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="148" spans="2:5" ht="15">
-      <c r="B148" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="C148" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D148" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E148" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B149" s="75" t="s">
-        <v>99</v>
-      </c>
-      <c r="C149" s="76" t="s">
-        <v>5</v>
-      </c>
-      <c r="D149" s="76" t="s">
-        <v>8</v>
-      </c>
-      <c r="E149" s="63">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B150" s="75"/>
-      <c r="C150" s="76"/>
-      <c r="D150" s="76"/>
-      <c r="E150" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" ht="15">
-      <c r="B151" s="75"/>
-      <c r="C151" s="76"/>
-      <c r="D151" s="76"/>
-      <c r="E151" s="63">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5" ht="15">
-      <c r="B152" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="C152" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="D152" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="E152" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="153" spans="2:5" ht="15">
-      <c r="B153" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="C153" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="D153" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="E153" s="63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="154" spans="2:5" ht="15">
-      <c r="B154" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="C154" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="D154" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="E154" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="155" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B155" s="75" t="s">
-        <v>107</v>
-      </c>
-      <c r="C155" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="D155" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="E155" s="63">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B156" s="75"/>
-      <c r="C156" s="76"/>
-      <c r="D156" s="76"/>
-      <c r="E156" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B157" s="75"/>
-      <c r="C157" s="76"/>
-      <c r="D157" s="76"/>
-      <c r="E157" s="63">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="158" spans="2:5" ht="15">
-      <c r="B158" s="75"/>
-      <c r="C158" s="76"/>
-      <c r="D158" s="76"/>
-      <c r="E158" s="63">
-        <v>450407</v>
-      </c>
-    </row>
-    <row r="159" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B159" s="75" t="s">
-        <v>108</v>
-      </c>
-      <c r="C159" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="D159" s="76" t="s">
-        <v>15</v>
-      </c>
-      <c r="E159" s="63">
-        <v>518841</v>
-      </c>
-    </row>
-    <row r="160" spans="2:5" ht="15">
-      <c r="B160" s="75"/>
-      <c r="C160" s="76"/>
-      <c r="D160" s="76"/>
-      <c r="E160" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="161" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B161" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="C161" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="D161" s="76" t="s">
-        <v>16</v>
-      </c>
-      <c r="E161" s="63">
-        <v>459419</v>
-      </c>
-    </row>
-    <row r="162" spans="2:5" ht="15">
-      <c r="B162" s="75"/>
-      <c r="C162" s="76"/>
-      <c r="D162" s="76"/>
-      <c r="E162" s="63">
-        <v>553643</v>
-      </c>
-    </row>
-    <row r="163" spans="2:5" s="55" customFormat="1" ht="15">
-      <c r="B163" s="75" t="s">
-        <v>109</v>
-      </c>
-      <c r="C163" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="D163" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="E163" s="63">
-        <v>518761</v>
-      </c>
-    </row>
-    <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1">
-      <c r="B164" s="75"/>
-      <c r="C164" s="76"/>
-      <c r="D164" s="76"/>
-      <c r="E164" s="63">
-        <v>450408</v>
-      </c>
-    </row>
-    <row r="165" spans="2:5" ht="15">
-      <c r="B165" s="75"/>
-      <c r="C165" s="76"/>
-      <c r="D165" s="76"/>
-      <c r="E165" s="63">
-        <v>421892</v>
-      </c>
-    </row>
-    <row r="166" spans="2:5" ht="15">
-      <c r="B166" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="C166" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="D166" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="E166" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="167" spans="2:5" ht="15">
-      <c r="B167" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="C167" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="D167" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="E167" s="63" t="s">
-        <v>41</v>
-      </c>
-    </row>
+    <row r="141" spans="2:5" ht="15"/>
+    <row r="142" spans="2:5" ht="14"/>
+    <row r="143" spans="2:5" ht="14"/>
+    <row r="144" spans="2:5" ht="14"/>
+    <row r="145" spans="2:5" ht="14"/>
+    <row r="146" spans="2:5" ht="15"/>
+    <row r="147" spans="2:5" ht="15"/>
+    <row r="148" spans="2:5" ht="15"/>
+    <row r="149" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="150" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="151" spans="2:5" ht="15"/>
+    <row r="152" spans="2:5" ht="15"/>
+    <row r="153" spans="2:5" ht="15"/>
+    <row r="154" spans="2:5" ht="15"/>
+    <row r="155" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="156" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
+    <row r="157" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
+    <row r="158" spans="2:5" ht="15"/>
+    <row r="159" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="160" spans="2:5" ht="15"/>
+    <row r="161" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="162" spans="2:5" ht="15"/>
+    <row r="163" spans="2:5" s="55" customFormat="1" ht="15"/>
+    <row r="164" spans="2:5" s="55" customFormat="1" ht="18" customHeight="1"/>
+    <row r="165" spans="2:5" ht="15"/>
+    <row r="166" spans="2:5" ht="15"/>
+    <row r="167" spans="2:5" ht="15"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D163:D165"/>
-    <mergeCell ref="C163:C165"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="D159:D160"/>
-    <mergeCell ref="C159:C160"/>
-    <mergeCell ref="B159:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="D161:D162"/>
-    <mergeCell ref="B149:B151"/>
-    <mergeCell ref="C149:C151"/>
-    <mergeCell ref="D149:D151"/>
-    <mergeCell ref="B155:B158"/>
-    <mergeCell ref="C155:C158"/>
-    <mergeCell ref="D155:D158"/>
-    <mergeCell ref="B141:E141"/>
     <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B85:C85"/>
@@ -2388,7 +1945,7 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="77" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>

</xml_diff>

<commit_message>
set no suggests values Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
@@ -309,6 +309,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="22">
     <font>
       <sz val="10"/>
@@ -453,7 +454,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,7 +466,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +585,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1029,7 +1030,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B32:E164"/>
+  <dimension ref="B32:D164"/>
   <sheetViews>
     <sheetView topLeftCell="A145" zoomScale="125" workbookViewId="0">
       <selection activeCell="C152" sqref="C152:C167"/>
@@ -1037,10 +1038,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="32" spans="2:3">
@@ -1404,10 +1405,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="17.33203125" style="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" style="22" width="17.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="22" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
@@ -1572,11 +1573,11 @@
       <c r="C13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="28">
-        <v>0</v>
-      </c>
-      <c r="E13" s="29">
-        <v>4500001</v>
+      <c r="D13" s="28" t="n">
+        <v>4500001.0</v>
+      </c>
+      <c r="E13" s="29" t="n">
+        <v>9.99999999E8</v>
       </c>
       <c r="F13" s="29">
         <v>0</v>
@@ -1623,11 +1624,11 @@
       <c r="C16" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="41">
-        <v>0</v>
-      </c>
-      <c r="E16" s="41">
-        <v>10000001</v>
+      <c r="D16" s="41" t="n">
+        <v>1.0000001E7</v>
+      </c>
+      <c r="E16" s="41" t="n">
+        <v>9.99999999E8</v>
       </c>
       <c r="F16" s="41">
         <v>0</v>
@@ -1753,11 +1754,11 @@
       <c r="C26" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="29">
-        <v>0</v>
-      </c>
-      <c r="E26" s="29">
-        <v>80000001</v>
+      <c r="D26" s="29" t="n">
+        <v>8000001.0</v>
+      </c>
+      <c r="E26" s="29" t="n">
+        <v>9.99999999E8</v>
       </c>
       <c r="F26" s="29">
         <v>0</v>
@@ -1822,11 +1823,11 @@
       <c r="C31" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="41">
-        <v>0</v>
-      </c>
-      <c r="E31" s="41">
-        <v>3000000</v>
+      <c r="D31" s="41" t="n">
+        <v>3000000.0</v>
+      </c>
+      <c r="E31" s="41" t="n">
+        <v>9.99999999E8</v>
       </c>
       <c r="F31" s="41">
         <v>0</v>
@@ -1839,11 +1840,11 @@
       <c r="C32" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="29">
-        <v>0</v>
-      </c>
-      <c r="E32" s="29">
-        <v>10000001</v>
+      <c r="D32" s="29" t="n">
+        <v>1.0000001E7</v>
+      </c>
+      <c r="E32" s="29" t="n">
+        <v>9.99999999E8</v>
       </c>
       <c r="F32" s="29">
         <v>0</v>

</xml_diff>

<commit_message>
create approvedCredit Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -8,20 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6915933-0829-5149-A1C9-F463A7945739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36230ABB-DA42-484E-8C1D-01BD455605FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="7" r:id="rId3"/>
+    <sheet name="VISA" sheetId="11" r:id="rId4"/>
+    <sheet name="MASTER" sheetId="12" r:id="rId5"/>
+    <sheet name="PLATINO" sheetId="8" r:id="rId6"/>
+    <sheet name="DORADO" sheetId="9" r:id="rId7"/>
+    <sheet name="PLATEADO" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
   <si>
     <t>RETURN</t>
   </si>
@@ -303,6 +317,135 @@
   </si>
   <si>
     <t>R180</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Rules response RangoValor(String cat, Double valor)</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>t == cat</t>
+  </si>
+  <si>
+    <t>String t</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Objecto</t>
+  </si>
+  <si>
+    <t>Datatype responseTest</t>
+  </si>
+  <si>
+    <t>new response(response)</t>
+  </si>
+  <si>
+    <t>Bolean responseTest</t>
+  </si>
+  <si>
+    <t>PLATINO</t>
+  </si>
+  <si>
+    <t>DORADO</t>
+  </si>
+  <si>
+    <t>PLATEADO</t>
+  </si>
+  <si>
+    <t>=OrderValidationPlatino(cat, valor)</t>
+  </si>
+  <si>
+    <t>=OrderValidationDorado(cat, valor)</t>
+  </si>
+  <si>
+    <t>=OrderValidationPlateado(cat, valor)</t>
+  </si>
+  <si>
+    <t>SimpleLookup Boolean OrderValidationPlatino(String categoria, Double monto)</t>
+  </si>
+  <si>
+    <t>Categoria / Monto_Autorizado</t>
+  </si>
+  <si>
+    <t>&lt;=1000</t>
+  </si>
+  <si>
+    <t>&gt;1000</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>SimpleLookup Boolean OrderValidationDorado(String categoria, Double monto)</t>
+  </si>
+  <si>
+    <t>SimpleLookup Boolean OrderValidationPlateado(String categoria, Double monto)</t>
+  </si>
+  <si>
+    <t>Datatype responseApprovedCredit</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>new responseApprovedCredit(amount)</t>
+  </si>
+  <si>
+    <t>Double amount</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>MASTERCARD</t>
+  </si>
+  <si>
+    <t>t == Franquicia</t>
+  </si>
+  <si>
+    <t>Rules responseApprovedCredit approvedCredit(String Franquicia, Double income)</t>
+  </si>
+  <si>
+    <t>=OrderValidationVisa(Franquicia, income)</t>
+  </si>
+  <si>
+    <t>=OrderValidationMastercard(Franquicia, income)</t>
+  </si>
+  <si>
+    <t>SimpleLookup Boolean OrderValidationVisa(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>Rules responseTest RangoValor(String cat, Double valor)</t>
+  </si>
+  <si>
+    <t>new responseTest(response)</t>
+  </si>
+  <si>
+    <t>Boolean response</t>
+  </si>
+  <si>
+    <t>SimpleLookup Boolean OrderValidationMastercard(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>SimpleLookup Double OrderValidationVisa(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>SimpleLookup Double OrderValidationMastercard(String categoria, Double income)</t>
   </si>
 </sst>
 </file>
@@ -310,7 +453,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -424,8 +567,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" rgb="FFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,12 +621,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921" rgb="9BBB59"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442" rgb="1F497D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921" rgb="1F497D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF538DD5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D9F1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -583,11 +780,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -670,27 +941,67 @@
     <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1032,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B32:D164"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152:C167"/>
+    <sheetView topLeftCell="A92" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1069,10 +1380,10 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="35" t="s">
+      <c r="B60" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="35"/>
+      <c r="C60" s="36"/>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="2" t="s">
@@ -1091,10 +1402,10 @@
       </c>
     </row>
     <row r="68" spans="2:3">
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C68" s="35"/>
+      <c r="C68" s="36"/>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="3" t="s">
@@ -1145,10 +1456,10 @@
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85" s="35" t="s">
+      <c r="B85" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C85" s="35"/>
+      <c r="C85" s="36"/>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" s="4" t="s">
@@ -1175,11 +1486,11 @@
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C94" s="35"/>
-      <c r="D94" s="35"/>
+      <c r="C94" s="36"/>
+      <c r="D94" s="36"/>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" s="5" t="s">
@@ -1303,10 +1614,10 @@
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="34" t="s">
+      <c r="B107" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C107" s="34"/>
+      <c r="C107" s="35"/>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="6" t="s">
@@ -1399,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F6224-7F2A-BA4D-ABDF-DEDD326C8E0B}">
   <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1412,13 +1723,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="23" t="s">
@@ -1532,16 +1843,16 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="37">
         <v>3000001</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="39">
         <v>4500000</v>
       </c>
       <c r="F10" s="27">
@@ -1549,19 +1860,19 @@
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="40"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="27">
         <v>450408</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="40"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="27">
         <v>518761</v>
       </c>
@@ -1573,11 +1884,11 @@
       <c r="C13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="28" t="n">
-        <v>4500001.0</v>
-      </c>
-      <c r="E13" s="29" t="n">
-        <v>9.99999999E8</v>
+      <c r="D13" s="28">
+        <v>4500001</v>
+      </c>
+      <c r="E13" s="29">
+        <v>999999999</v>
       </c>
       <c r="F13" s="29">
         <v>0</v>
@@ -1621,16 +1932,16 @@
       <c r="B16" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="41" t="n">
-        <v>1.0000001E7</v>
-      </c>
-      <c r="E16" s="41" t="n">
-        <v>9.99999999E8</v>
-      </c>
-      <c r="F16" s="41">
+      <c r="D16" s="34">
+        <v>10000001</v>
+      </c>
+      <c r="E16" s="34">
+        <v>999999999</v>
+      </c>
+      <c r="F16" s="34">
         <v>0</v>
       </c>
     </row>
@@ -1652,16 +1963,16 @@
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="40">
         <v>2000001</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="40">
         <v>4000000</v>
       </c>
       <c r="F18" s="31">
@@ -1669,43 +1980,43 @@
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="31">
         <v>450408</v>
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="31">
         <v>421892</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="31">
         <v>450407</v>
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="40">
         <v>4000001</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="40">
         <v>6000000</v>
       </c>
       <c r="F22" s="31">
@@ -1713,25 +2024,25 @@
       </c>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="31">
         <v>450408</v>
       </c>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="40">
         <v>6000001</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="40">
         <v>8000000</v>
       </c>
       <c r="F24" s="31">
@@ -1739,10 +2050,10 @@
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="31">
         <v>553643</v>
       </c>
@@ -1754,27 +2065,27 @@
       <c r="C26" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="29" t="n">
-        <v>8000001.0</v>
-      </c>
-      <c r="E26" s="29" t="n">
-        <v>9.99999999E8</v>
+      <c r="D26" s="29">
+        <v>8000001</v>
+      </c>
+      <c r="E26" s="29">
+        <v>999999999</v>
       </c>
       <c r="F26" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D27" s="41">
         <v>300000</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="41">
         <v>10000000</v>
       </c>
       <c r="F27" s="30">
@@ -1782,19 +2093,19 @@
       </c>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="30">
         <v>450408</v>
       </c>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="30">
         <v>421892</v>
       </c>
@@ -1817,19 +2128,19 @@
       </c>
     </row>
     <row r="31" spans="2:6" s="22" customFormat="1">
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="41" t="n">
-        <v>3000000.0</v>
-      </c>
-      <c r="E31" s="41" t="n">
-        <v>9.99999999E8</v>
-      </c>
-      <c r="F31" s="41">
+      <c r="D31" s="34">
+        <v>3000000</v>
+      </c>
+      <c r="E31" s="34">
+        <v>999999999</v>
+      </c>
+      <c r="F31" s="34">
         <v>0</v>
       </c>
     </row>
@@ -1840,11 +2151,11 @@
       <c r="C32" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="29" t="n">
-        <v>1.0000001E7</v>
-      </c>
-      <c r="E32" s="29" t="n">
-        <v>9.99999999E8</v>
+      <c r="D32" s="29">
+        <v>10000001</v>
+      </c>
+      <c r="E32" s="29">
+        <v>999999999</v>
       </c>
       <c r="F32" s="29">
         <v>0</v>
@@ -1869,11 +2180,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E18:E21"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E27:E29"/>
@@ -1890,8 +2196,479 @@
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E18:E21"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CBDFE8-F62E-B24F-B8E6-13E2DE95B141}">
+  <dimension ref="B5:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.1640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4">
+      <c r="B5" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="49"/>
+      <c r="C6" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="43"/>
+      <c r="C7" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="43"/>
+      <c r="C8" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="42"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="49"/>
+      <c r="C24" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="43"/>
+      <c r="C25" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="43"/>
+      <c r="C26" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="51"/>
+      <c r="D27" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B33:C33"/>
+  </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE1AECC-4D49-FB47-B6A5-D545314CE96F}">
+  <dimension ref="B4:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.83203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4">
+      <c r="B4" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="55">
+        <v>2000</v>
+      </c>
+      <c r="D6" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="C6:D6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B423DEF3-23F4-5B49-820F-FDF0C968F35B}">
+  <dimension ref="B3:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="3" customWidth="true" width="25.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="B3" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="55">
+        <v>5000</v>
+      </c>
+      <c r="D5" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5384800-4FC3-7C41-B487-4C00885AA4B8}">
+  <dimension ref="B5:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.1640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4">
+      <c r="B5" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC78498E-2B9B-5D40-87EE-D6BEBAA1F919}">
+  <dimension ref="B5:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.5" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4">
+      <c r="B5" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43556C87-DDB2-B149-ACDD-211F0452386D}">
+  <dimension ref="B5:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="29.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.5" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4">
+      <c r="B5" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
verificación de cupo TC Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -8,19 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandelahoz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36230ABB-DA42-484E-8C1D-01BD455605FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D302CB9-24F9-404B-8D51-A4CF7692A769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2440" windowWidth="27320" windowHeight="14900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rules" sheetId="5" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="7" r:id="rId3"/>
-    <sheet name="VISA" sheetId="11" r:id="rId4"/>
-    <sheet name="MASTER" sheetId="12" r:id="rId5"/>
-    <sheet name="PLATINO" sheetId="8" r:id="rId6"/>
-    <sheet name="DORADO" sheetId="9" r:id="rId7"/>
-    <sheet name="PLATEADO" sheetId="10" r:id="rId8"/>
+    <sheet name="BasicRules" sheetId="5" r:id="rId1"/>
+    <sheet name="suggestCards" sheetId="6" r:id="rId2"/>
+    <sheet name="aprovedCredit" sheetId="7" r:id="rId3"/>
+    <sheet name="Franquicias" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
   <si>
     <t>RETURN</t>
   </si>
@@ -322,21 +318,9 @@
     <t>Double</t>
   </si>
   <si>
-    <t>response</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Rules response RangoValor(String cat, Double valor)</t>
-  </si>
-  <si>
     <t>RET</t>
   </si>
   <si>
-    <t>t == cat</t>
-  </si>
-  <si>
     <t>String t</t>
   </si>
   <si>
@@ -346,57 +330,9 @@
     <t>Objecto</t>
   </si>
   <si>
-    <t>Datatype responseTest</t>
-  </si>
-  <si>
-    <t>new response(response)</t>
-  </si>
-  <si>
-    <t>Bolean responseTest</t>
-  </si>
-  <si>
-    <t>PLATINO</t>
-  </si>
-  <si>
-    <t>DORADO</t>
-  </si>
-  <si>
-    <t>PLATEADO</t>
-  </si>
-  <si>
-    <t>=OrderValidationPlatino(cat, valor)</t>
-  </si>
-  <si>
-    <t>=OrderValidationDorado(cat, valor)</t>
-  </si>
-  <si>
-    <t>=OrderValidationPlateado(cat, valor)</t>
-  </si>
-  <si>
-    <t>SimpleLookup Boolean OrderValidationPlatino(String categoria, Double monto)</t>
-  </si>
-  <si>
     <t>Categoria / Monto_Autorizado</t>
   </si>
   <si>
-    <t>&lt;=1000</t>
-  </si>
-  <si>
-    <t>&gt;1000</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>SimpleLookup Boolean OrderValidationDorado(String categoria, Double monto)</t>
-  </si>
-  <si>
-    <t>SimpleLookup Boolean OrderValidationPlateado(String categoria, Double monto)</t>
-  </si>
-  <si>
     <t>Datatype responseApprovedCredit</t>
   </si>
   <si>
@@ -421,39 +357,149 @@
     <t>Rules responseApprovedCredit approvedCredit(String Franquicia, Double income)</t>
   </si>
   <si>
-    <t>=OrderValidationVisa(Franquicia, income)</t>
-  </si>
-  <si>
-    <t>=OrderValidationMastercard(Franquicia, income)</t>
-  </si>
-  <si>
-    <t>SimpleLookup Boolean OrderValidationVisa(String categoria, Double income)</t>
-  </si>
-  <si>
-    <t>Rules responseTest RangoValor(String cat, Double valor)</t>
-  </si>
-  <si>
-    <t>new responseTest(response)</t>
-  </si>
-  <si>
-    <t>Boolean response</t>
-  </si>
-  <si>
-    <t>SimpleLookup Boolean OrderValidationMastercard(String categoria, Double income)</t>
-  </si>
-  <si>
-    <t>SimpleLookup Double OrderValidationVisa(String categoria, Double income)</t>
-  </si>
-  <si>
-    <t>SimpleLookup Double OrderValidationMastercard(String categoria, Double income)</t>
+    <t>AMERICAN_EXPRESS</t>
+  </si>
+  <si>
+    <t>DINERS_CLUB</t>
+  </si>
+  <si>
+    <t>SimpleLookup Double OrderValidationAmerican(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>&lt;=500000</t>
+  </si>
+  <si>
+    <t>&lt;750000</t>
+  </si>
+  <si>
+    <t>&lt;1500000</t>
+  </si>
+  <si>
+    <t>&gt;=750001</t>
+  </si>
+  <si>
+    <t>&gt;=1500001</t>
+  </si>
+  <si>
+    <t>&lt;3000000</t>
+  </si>
+  <si>
+    <t>&gt;=3000001</t>
+  </si>
+  <si>
+    <t>&lt;10000000</t>
+  </si>
+  <si>
+    <t>=income*2</t>
+  </si>
+  <si>
+    <t>=income*1</t>
+  </si>
+  <si>
+    <t>=income*1.5</t>
+  </si>
+  <si>
+    <t>=income*1.2</t>
+  </si>
+  <si>
+    <t>=income*0.5</t>
+  </si>
+  <si>
+    <t>=income*0.7</t>
+  </si>
+  <si>
+    <t>=income*1.3</t>
+  </si>
+  <si>
+    <t>&gt;=1</t>
+  </si>
+  <si>
+    <t>SimpleRules Double validateMaxLimit(Double calc)</t>
+  </si>
+  <si>
+    <t>=calc</t>
+  </si>
+  <si>
+    <t>&lt;1</t>
+  </si>
+  <si>
+    <t>Max Limit (m COP)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2" tint="-0.749992370372631"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>SimpleRules Double</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>MaxLimitCreditCard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> ()</t>
+    </r>
+  </si>
+  <si>
+    <t>SimpleLookup Double aprovedVisa(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>SimpleLookup Double aprovedMastercard(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>SimpleLookup Double aprovedDiners(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedVisa(Franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedMastercard(Franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedDiners(Franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedAmerican(Franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>SimpleLookup Double aprovedAmerican(String categoria, Double income)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="24">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$$-240A]\ #,##0.00"/>
+  </numFmts>
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -575,12 +621,54 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,13 +715,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921" rgb="9BBB59"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,26 +737,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF538DD5"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5D9F1"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -819,46 +889,60 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -944,68 +1028,73 @@
     <xf numFmtId="0" fontId="21" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_EPLI rater" xfId="1" xr:uid="{AC981B7D-DB10-4341-9511-47A22FCD7E79}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1343,13 +1432,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B32:D164"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+    <sheetView topLeftCell="A112" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="25.1640625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="27.83203125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
@@ -1380,10 +1469,10 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="36"/>
+      <c r="C60" s="44"/>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="2" t="s">
@@ -1402,10 +1491,10 @@
       </c>
     </row>
     <row r="68" spans="2:3">
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C68" s="36"/>
+      <c r="C68" s="44"/>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" s="3" t="s">
@@ -1456,10 +1545,10 @@
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C85" s="36"/>
+      <c r="C85" s="44"/>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" s="4" t="s">
@@ -1486,11 +1575,11 @@
       </c>
     </row>
     <row r="94" spans="2:4">
-      <c r="B94" s="36" t="s">
+      <c r="B94" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
     </row>
     <row r="95" spans="2:4">
       <c r="B95" s="5" t="s">
@@ -1614,10 +1703,10 @@
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="35" t="s">
+      <c r="B107" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C107" s="35"/>
+      <c r="C107" s="43"/>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="6" t="s">
@@ -1683,7 +1772,69 @@
         <v>57</v>
       </c>
     </row>
-    <row r="133" s="22" customFormat="1"/>
+    <row r="121" spans="2:3">
+      <c r="B121" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C121" s="51"/>
+    </row>
+    <row r="122" spans="2:3">
+      <c r="B122" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C122" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3">
+      <c r="B127" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C127" s="43"/>
+    </row>
+    <row r="128" spans="2:3" ht="14" thickBot="1">
+      <c r="B128" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" ht="14" thickTop="1">
+      <c r="B129" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C129" s="62" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3">
+      <c r="B130" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C130" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" s="22" customFormat="1">
+      <c r="B133"/>
+      <c r="C133"/>
+    </row>
+    <row r="135" spans="2:3" ht="20" thickBot="1">
+      <c r="B135" s="63" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" ht="20" thickBot="1">
+      <c r="B136" s="64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" ht="15" thickBot="1">
+      <c r="B137" s="65">
+        <v>17000000</v>
+      </c>
+    </row>
     <row r="149" s="22" customFormat="1"/>
     <row r="150" s="22" customFormat="1"/>
     <row r="155" s="22" customFormat="1"/>
@@ -1694,7 +1845,9 @@
     <row r="163" s="22" customFormat="1"/>
     <row r="164" s="22" customFormat="1" ht="18" customHeight="1"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B127:C127"/>
     <mergeCell ref="B107:C107"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B68:C68"/>
@@ -1710,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F6224-7F2A-BA4D-ABDF-DEDD326C8E0B}">
   <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1723,13 +1876,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="23" t="s">
@@ -1843,16 +1996,16 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="47">
         <v>3000001</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="49">
         <v>4500000</v>
       </c>
       <c r="F10" s="27">
@@ -1860,19 +2013,19 @@
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="39"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="27">
         <v>450408</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="39"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="27">
         <v>518761</v>
       </c>
@@ -1963,16 +2116,16 @@
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="45">
         <v>2000001</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="45">
         <v>4000000</v>
       </c>
       <c r="F18" s="31">
@@ -1980,43 +2133,43 @@
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="31">
         <v>450408</v>
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="31">
         <v>421892</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="31">
         <v>450407</v>
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="45">
         <v>4000001</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="45">
         <v>6000000</v>
       </c>
       <c r="F22" s="31">
@@ -2024,25 +2177,25 @@
       </c>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
       <c r="F23" s="31">
         <v>450408</v>
       </c>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="45">
         <v>6000001</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="45">
         <v>8000000</v>
       </c>
       <c r="F24" s="31">
@@ -2050,10 +2203,10 @@
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="31">
         <v>553643</v>
       </c>
@@ -2076,16 +2229,16 @@
       </c>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="46">
         <v>300000</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="46">
         <v>10000000</v>
       </c>
       <c r="F27" s="30">
@@ -2093,19 +2246,19 @@
       </c>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="30">
         <v>450408</v>
       </c>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="30">
         <v>421892</v>
       </c>
@@ -2180,6 +2333,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E18:E21"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E27:E29"/>
@@ -2196,11 +2354,6 @@
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E18:E21"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2209,210 +2362,147 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CBDFE8-F62E-B24F-B8E6-13E2DE95B141}">
-  <dimension ref="B5:D34"/>
+  <dimension ref="A6:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="101.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4">
-      <c r="B5" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="49"/>
-      <c r="C6" s="49" t="s">
+    <row r="6" spans="1:4">
+      <c r="B6" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="54"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D7" s="38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="35"/>
+      <c r="C8" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="35"/>
+      <c r="C9" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="39" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="43"/>
-      <c r="C7" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="43"/>
-      <c r="C8" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="50" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="25" t="s">
+    <row r="11" spans="1:4">
+      <c r="B11" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="45" t="s">
+      <c r="C11" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="25" t="s">
+      <c r="D13" s="37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="22"/>
+      <c r="B14" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="45" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="42"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="49"/>
-      <c r="C24" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="49" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="43"/>
-      <c r="C25" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="43"/>
-      <c r="C26" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="50" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="22"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>121</v>
-      </c>
+      <c r="D14" s="37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="22"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="F17" s="61"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="D18" s="22"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="F20" s="61"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="F21" s="61"/>
+    </row>
+    <row r="26" spans="1:6" s="22" customFormat="1">
+      <c r="A26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:6" s="22" customFormat="1">
+      <c r="A27"/>
+      <c r="D27"/>
+      <c r="E27"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B33:C33"/>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2421,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE1AECC-4D49-FB47-B6A5-D545314CE96F}">
-  <dimension ref="B4:D6"/>
+  <dimension ref="B4:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2434,240 +2524,298 @@
     <col min="4" max="4" customWidth="true" width="23.83203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4">
-      <c r="B4" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="54" t="s">
+    <row r="4" spans="2:10">
+      <c r="B4" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="G5" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="60"/>
+      <c r="E6" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="60"/>
+      <c r="G6" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="60"/>
+      <c r="I6" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="60"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="F17" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="41" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="53" t="s">
+      <c r="H17" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="60"/>
+      <c r="E18" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="55">
-        <v>2000</v>
-      </c>
-      <c r="D6" s="56"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="60"/>
+      <c r="I18" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="60"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="60"/>
+      <c r="E32" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="60"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H43" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="60"/>
+      <c r="E44" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="60"/>
+      <c r="G44" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="H44" s="60"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B4:D4"/>
+  <mergeCells count="17">
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="B30:F30"/>
     <mergeCell ref="C6:D6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B423DEF3-23F4-5B49-820F-FDF0C968F35B}">
-  <dimension ref="B3:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="3" customWidth="true" width="25.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:4">
-      <c r="B3" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="55">
-        <v>5000</v>
-      </c>
-      <c r="D5" s="56"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="C5:D5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5384800-4FC3-7C41-B487-4C00885AA4B8}">
-  <dimension ref="B5:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="28.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.1640625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="2:4">
-      <c r="B5" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="56"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:D7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC78498E-2B9B-5D40-87EE-D6BEBAA1F919}">
-  <dimension ref="B5:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.1640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.5" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="2:4">
-      <c r="B5" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:D5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43556C87-DDB2-B149-ACDD-211F0452386D}">
-  <dimension ref="B5:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="29.83203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="27.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="32.5" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="2:4">
-      <c r="B5" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="58" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="63"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix response approvedCredit Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="141">
   <si>
     <t>RETURN</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>SimpleLookup Double aprovedAmerican(String categoria, Double income)</t>
+  </si>
+  <si>
+    <t>Rules Double approvedCredit(String Franquicia, Double income)</t>
   </si>
 </sst>
 </file>
@@ -715,13 +718,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.39997558519241921" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2373,12 +2376,12 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="32.83203125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="101.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:4">
       <c r="B6" s="52" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54"/>
@@ -2397,18 +2400,14 @@
       <c r="C8" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>102</v>
-      </c>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="35"/>
       <c r="C9" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>103</v>
-      </c>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="39" t="s">

</xml_diff>

<commit_message>
Fix response appovedCredit Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
   <si>
     <t>RETURN</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t xml:space="preserve">new </t>
+  </si>
+  <si>
+    <t>Rules Double[] approvedCredit(String Franquicia, Double income)</t>
   </si>
 </sst>
 </file>
@@ -2384,7 +2387,7 @@
   <sheetData>
     <row r="6" spans="1:4">
       <c r="B6" s="52" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54"/>
@@ -2403,18 +2406,14 @@
       <c r="C8" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>102</v>
-      </c>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="35"/>
       <c r="C9" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>103</v>
-      </c>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="39" t="s">

</xml_diff>

<commit_message>
test fix approvalCredit Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="147">
   <si>
     <t>RETURN</t>
   </si>
@@ -499,6 +499,18 @@
   </si>
   <si>
     <t>Rules Double[] approvedCredit(String Franquicia, Double income)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Double[] approvedCredit(String Franquicia, Double income)</t>
+  </si>
+  <si>
+    <t>Rules resApprovedCredit approvedCredit(String Franquicia, Double income)</t>
+  </si>
+  <si>
+    <t>new resApprovedCredit(amount)</t>
+  </si>
+  <si>
+    <t>Datatype resApprovedCredit</t>
   </si>
 </sst>
 </file>
@@ -747,7 +759,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -946,12 +958,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1100,6 +1130,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1439,7 +1470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B32:D164"/>
+  <dimension ref="B32:D167"/>
   <sheetViews>
     <sheetView topLeftCell="A112" zoomScale="125" workbookViewId="0">
       <selection activeCell="C124" sqref="C124"/>
@@ -1853,8 +1884,22 @@
     <row r="161" s="22" customFormat="1"/>
     <row r="163" s="22" customFormat="1"/>
     <row r="164" s="22" customFormat="1" ht="18" customHeight="1"/>
+    <row r="166">
+      <c r="B166" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="C166" s="66"/>
+    </row>
+    <row r="167">
+      <c r="B167" t="s" s="66">
+        <v>94</v>
+      </c>
+      <c r="C167" t="s" s="66">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B121:C121"/>
     <mergeCell ref="B127:C127"/>
     <mergeCell ref="B107:C107"/>
@@ -1862,6 +1907,7 @@
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B166:C166"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2387,7 +2433,7 @@
   <sheetData>
     <row r="6" spans="1:4">
       <c r="B6" s="52" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54"/>
@@ -2406,14 +2452,18 @@
       <c r="C8" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="25" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="35"/>
       <c r="C9" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="25" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="39" t="s">

</xml_diff>

<commit_message>
FIx approvedCredit Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="148">
   <si>
     <t>RETURN</t>
   </si>
@@ -511,6 +511,9 @@
   </si>
   <si>
     <t>Datatype resApprovedCredit</t>
+  </si>
+  <si>
+    <t>Rules resApprovedCredit approvedCredit(Double income, String Franquicia)</t>
   </si>
 </sst>
 </file>
@@ -2433,7 +2436,7 @@
   <sheetData>
     <row r="6" spans="1:4">
       <c r="B6" s="52" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54"/>

</xml_diff>

<commit_message>
Fix paramaters approvedCredit Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="154">
   <si>
     <t>RETURN</t>
   </si>
@@ -514,6 +514,24 @@
   </si>
   <si>
     <t>Rules resApprovedCredit approvedCredit(Double income, String Franquicia)</t>
+  </si>
+  <si>
+    <t>Rules resApprovedCredit approvedCredit(Double income, String franquicia)</t>
+  </si>
+  <si>
+    <t>t == franquicia</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedVisa(franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedMastercard(franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedDiners(franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedAmerican(franquicia, income) / MaxLimitCreditCard() ) )</t>
   </si>
 </sst>
 </file>
@@ -2436,7 +2454,7 @@
   <sheetData>
     <row r="6" spans="1:4">
       <c r="B6" s="52" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54"/>
@@ -2453,7 +2471,7 @@
     <row r="8" spans="1:4">
       <c r="B8" s="35"/>
       <c r="C8" s="25" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>145</v>
@@ -2485,7 +2503,7 @@
         <v>104</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2496,7 +2514,7 @@
         <v>105</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2507,7 +2525,7 @@
         <v>109</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2519,7 +2537,7 @@
         <v>108</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:4">

</xml_diff>

<commit_message>
create getSuggestCards Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/BBVA_Rules/Main.xlsx
+++ b/DESIGN/rules/BBVA_Rules/Main.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="155">
   <si>
     <t>RETURN</t>
   </si>
@@ -532,6 +532,9 @@
   </si>
   <si>
     <t>=( MaxLimitCreditCard() * validateMaxLimit(aprovedAmerican(franquicia, income) / MaxLimitCreditCard() ) )</t>
+  </si>
+  <si>
+    <t>Rules String[] getSuggestCards (String situation, Double income)</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B32:D167"/>
+  <dimension ref="B32:F200"/>
   <sheetViews>
     <sheetView topLeftCell="A112" zoomScale="125" workbookViewId="0">
       <selection activeCell="C124" sqref="C124"/>
@@ -1919,8 +1922,536 @@
         <v>101</v>
       </c>
     </row>
+    <row r="169">
+      <c r="B169" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="C169" s="48"/>
+      <c r="D169" s="48"/>
+      <c r="E169" s="48"/>
+      <c r="F169" s="48"/>
+    </row>
+    <row r="170">
+      <c r="B170" t="s" s="23">
+        <v>61</v>
+      </c>
+      <c r="C170" t="s" s="23">
+        <v>62</v>
+      </c>
+      <c r="D170" t="s" s="23">
+        <v>63</v>
+      </c>
+      <c r="E170" t="s" s="23">
+        <v>70</v>
+      </c>
+      <c r="F170" t="s" s="23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" s="25"/>
+      <c r="C171" t="s" s="25">
+        <v>3</v>
+      </c>
+      <c r="D171" t="s" s="25">
+        <v>72</v>
+      </c>
+      <c r="E171" t="s" s="25">
+        <v>71</v>
+      </c>
+      <c r="F171" s="25"/>
+    </row>
+    <row r="172">
+      <c r="B172" s="25"/>
+      <c r="C172" t="s" s="25">
+        <v>73</v>
+      </c>
+      <c r="D172" t="s" s="25">
+        <v>66</v>
+      </c>
+      <c r="E172" t="s" s="25">
+        <v>67</v>
+      </c>
+      <c r="F172" s="25"/>
+    </row>
+    <row r="173">
+      <c r="B173" t="s" s="24">
+        <v>61</v>
+      </c>
+      <c r="C173" t="s" s="24">
+        <v>76</v>
+      </c>
+      <c r="D173" t="s" s="24">
+        <v>77</v>
+      </c>
+      <c r="E173" t="s" s="24">
+        <v>78</v>
+      </c>
+      <c r="F173" t="s" s="24">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="C174" t="s" s="26">
+        <v>4</v>
+      </c>
+      <c r="D174" t="n" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="E174" t="n" s="27">
+        <v>1000000.0</v>
+      </c>
+      <c r="F174" t="s" s="27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="s" s="26">
+        <v>69</v>
+      </c>
+      <c r="C175" t="s" s="26">
+        <v>4</v>
+      </c>
+      <c r="D175" t="n" s="26">
+        <v>1000001.0</v>
+      </c>
+      <c r="E175" t="n" s="27">
+        <v>2000000.0</v>
+      </c>
+      <c r="F175" t="s" s="27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" t="s" s="26">
+        <v>74</v>
+      </c>
+      <c r="C176" t="s" s="26">
+        <v>4</v>
+      </c>
+      <c r="D176" t="n" s="26">
+        <v>2000001.0</v>
+      </c>
+      <c r="E176" t="n" s="27">
+        <v>3000000.0</v>
+      </c>
+      <c r="F176" t="s" s="27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C177" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D177" t="n" s="47">
+        <v>3000001.0</v>
+      </c>
+      <c r="E177" t="n" s="49">
+        <v>4500000.0</v>
+      </c>
+      <c r="F177" t="n" s="27">
+        <v>421892.0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C178" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" s="47" t="n">
+        <v>3000001.0</v>
+      </c>
+      <c r="E178" s="49" t="n">
+        <v>4500000.0</v>
+      </c>
+      <c r="F178" t="n" s="27">
+        <v>450408.0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="B179" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C179" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D179" s="47" t="n">
+        <v>3000001.0</v>
+      </c>
+      <c r="E179" s="49" t="n">
+        <v>4500000.0</v>
+      </c>
+      <c r="F179" t="n" s="27">
+        <v>518761.0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="s" s="28">
+        <v>79</v>
+      </c>
+      <c r="C180" t="s" s="28">
+        <v>4</v>
+      </c>
+      <c r="D180" t="n" s="28">
+        <v>4500001.0</v>
+      </c>
+      <c r="E180" t="n" s="29">
+        <v>9.99999999E8</v>
+      </c>
+      <c r="F180" t="n" s="29">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="B181" t="s" s="30">
+        <v>80</v>
+      </c>
+      <c r="C181" t="s" s="30">
+        <v>5</v>
+      </c>
+      <c r="D181" t="n" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="E181" t="n" s="30">
+        <v>1000000.0</v>
+      </c>
+      <c r="F181" t="s" s="30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="B182" t="s" s="33">
+        <v>81</v>
+      </c>
+      <c r="C182" t="s" s="30">
+        <v>5</v>
+      </c>
+      <c r="D182" t="n" s="30">
+        <v>1000001.0</v>
+      </c>
+      <c r="E182" t="n" s="30">
+        <v>1.0E7</v>
+      </c>
+      <c r="F182" t="s" s="30">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="B183" t="s" s="33">
+        <v>82</v>
+      </c>
+      <c r="C183" t="s" s="34">
+        <v>5</v>
+      </c>
+      <c r="D183" t="n" s="34">
+        <v>1.0000001E7</v>
+      </c>
+      <c r="E183" t="n" s="34">
+        <v>9.99999999E8</v>
+      </c>
+      <c r="F183" t="n" s="34">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="B184" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C184" t="s" s="31">
+        <v>6</v>
+      </c>
+      <c r="D184" t="n" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="E184" t="n" s="31">
+        <v>2000000.0</v>
+      </c>
+      <c r="F184" t="s" s="31">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="B185" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C185" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" t="n" s="45">
+        <v>2000001.0</v>
+      </c>
+      <c r="E185" t="n" s="45">
+        <v>4000000.0</v>
+      </c>
+      <c r="F185" t="n" s="31">
+        <v>518761.0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="B186" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C186" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D186" s="45" t="n">
+        <v>2000001.0</v>
+      </c>
+      <c r="E186" s="45" t="n">
+        <v>4000000.0</v>
+      </c>
+      <c r="F186" t="n" s="31">
+        <v>450408.0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C187" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" s="45" t="n">
+        <v>2000001.0</v>
+      </c>
+      <c r="E187" s="45" t="n">
+        <v>4000000.0</v>
+      </c>
+      <c r="F187" t="n" s="31">
+        <v>421892.0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="B188" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C188" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D188" s="45" t="n">
+        <v>2000001.0</v>
+      </c>
+      <c r="E188" s="45" t="n">
+        <v>4000000.0</v>
+      </c>
+      <c r="F188" t="n" s="31">
+        <v>450407.0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C189" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" t="n" s="45">
+        <v>4000001.0</v>
+      </c>
+      <c r="E189" t="n" s="45">
+        <v>6000000.0</v>
+      </c>
+      <c r="F189" t="n" s="31">
+        <v>518841.0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C190" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D190" s="45" t="n">
+        <v>4000001.0</v>
+      </c>
+      <c r="E190" s="45" t="n">
+        <v>6000000.0</v>
+      </c>
+      <c r="F190" t="n" s="31">
+        <v>450408.0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C191" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D191" t="n" s="45">
+        <v>6000001.0</v>
+      </c>
+      <c r="E191" t="n" s="45">
+        <v>8000000.0</v>
+      </c>
+      <c r="F191" t="n" s="31">
+        <v>459419.0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C192" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" s="45" t="n">
+        <v>6000001.0</v>
+      </c>
+      <c r="E192" s="45" t="n">
+        <v>8000000.0</v>
+      </c>
+      <c r="F192" t="n" s="31">
+        <v>553643.0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" t="s" s="29">
+        <v>87</v>
+      </c>
+      <c r="C193" t="s" s="29">
+        <v>6</v>
+      </c>
+      <c r="D193" t="n" s="29">
+        <v>8000001.0</v>
+      </c>
+      <c r="E193" t="n" s="29">
+        <v>9.99999999E8</v>
+      </c>
+      <c r="F193" t="n" s="29">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="B194" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C194" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D194" t="n" s="46">
+        <v>300000.0</v>
+      </c>
+      <c r="E194" t="n" s="46">
+        <v>1.0E7</v>
+      </c>
+      <c r="F194" t="n" s="30">
+        <v>518761.0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C195" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195" s="46" t="n">
+        <v>300000.0</v>
+      </c>
+      <c r="E195" s="46" t="n">
+        <v>1.0E7</v>
+      </c>
+      <c r="F195" t="n" s="30">
+        <v>450408.0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="B196" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C196" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D196" s="46" t="n">
+        <v>300000.0</v>
+      </c>
+      <c r="E196" s="46" t="n">
+        <v>1.0E7</v>
+      </c>
+      <c r="F196" t="n" s="30">
+        <v>421892.0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="B197" t="s" s="30">
+        <v>90</v>
+      </c>
+      <c r="C197" t="s" s="30">
+        <v>7</v>
+      </c>
+      <c r="D197" t="n" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="E197" t="n" s="30">
+        <v>2999999.0</v>
+      </c>
+      <c r="F197" t="s" s="30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="B198" t="s" s="34">
+        <v>91</v>
+      </c>
+      <c r="C198" t="s" s="34">
+        <v>7</v>
+      </c>
+      <c r="D198" t="n" s="34">
+        <v>3000000.0</v>
+      </c>
+      <c r="E198" t="n" s="34">
+        <v>9.99999999E8</v>
+      </c>
+      <c r="F198" t="n" s="34">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="B199" t="s" s="32">
+        <v>92</v>
+      </c>
+      <c r="C199" t="s" s="29">
+        <v>8</v>
+      </c>
+      <c r="D199" t="n" s="29">
+        <v>1.0000001E7</v>
+      </c>
+      <c r="E199" t="n" s="29">
+        <v>9.99999999E8</v>
+      </c>
+      <c r="F199" t="n" s="29">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="B200" t="s" s="29">
+        <v>93</v>
+      </c>
+      <c r="C200" t="s" s="32">
+        <v>8</v>
+      </c>
+      <c r="D200" t="n" s="32">
+        <v>0.0</v>
+      </c>
+      <c r="E200" t="n" s="32">
+        <v>1.0E7</v>
+      </c>
+      <c r="F200" t="s" s="32">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="29">
     <mergeCell ref="B121:C121"/>
     <mergeCell ref="B127:C127"/>
     <mergeCell ref="B107:C107"/>
@@ -1929,6 +2460,27 @@
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B177:B179"/>
+    <mergeCell ref="B185:B188"/>
+    <mergeCell ref="B189:B190"/>
+    <mergeCell ref="B191:B192"/>
+    <mergeCell ref="B194:B196"/>
+    <mergeCell ref="C177:C179"/>
+    <mergeCell ref="C185:C188"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="C194:C196"/>
+    <mergeCell ref="D177:D179"/>
+    <mergeCell ref="D185:D188"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="D191:D192"/>
+    <mergeCell ref="D194:D196"/>
+    <mergeCell ref="E177:E179"/>
+    <mergeCell ref="E185:E188"/>
+    <mergeCell ref="E189:E190"/>
+    <mergeCell ref="E191:E192"/>
+    <mergeCell ref="E194:E196"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>